<commit_message>
Update Progen same with inventory system
</commit_message>
<xml_diff>
--- a/Issued Report.xlsx
+++ b/Issued Report.xlsx
@@ -15,9 +15,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="44">
-  <si>
-    <t>CENTRAL NEGROS POWER RELIABILITY, INC.</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="46">
+  <si>
+    <t>PROGEN DIESEL TECH</t>
   </si>
   <si>
     <t>Purok San Jose, Brgy. Calumangan, Bago City</t>
@@ -35,13 +35,25 @@
     <t>TO</t>
   </si>
   <si>
-    <t>2019-01-01</t>
+    <t>2020-03-01</t>
   </si>
   <si>
     <t>FROM</t>
   </si>
   <si>
-    <t>2019-03-28</t>
+    <t>2020-04-27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total Cost w/ PR: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total Number of Items w/ PR w/o Cost: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total Cost of WH Stocks: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total Number of Items from WH Stocks w/o Cost: </t>
   </si>
   <si>
     <t>Warehouse</t>
@@ -62,6 +74,9 @@
     <t>Issue Date</t>
   </si>
   <si>
+    <t>MIF No.</t>
+  </si>
+  <si>
     <t>PR No.</t>
   </si>
   <si>
@@ -71,13 +86,16 @@
     <t>Item Description</t>
   </si>
   <si>
+    <t>Total Qty Issued</t>
+  </si>
+  <si>
     <t>UoM</t>
   </si>
   <si>
-    <t>Total Qty Received</t>
-  </si>
-  <si>
-    <t>Supplier</t>
+    <t>Unit Cost</t>
+  </si>
+  <si>
+    <t>Total Cost</t>
   </si>
   <si>
     <t>Department</t>
@@ -92,44 +110,32 @@
     <t>Frequency</t>
   </si>
   <si>
-    <t>2019-01-31</t>
-  </si>
-  <si>
-    <t>pr1001</t>
-  </si>
-  <si>
-    <t>BUI-MAT_1023</t>
-  </si>
-  <si>
-    <t>Cement, Portland</t>
-  </si>
-  <si>
-    <t>bag/s</t>
-  </si>
-  <si>
-    <t>A.C. Parts Merchandising</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Accounting Department
+    <t>2020-04-22</t>
+  </si>
+  <si>
+    <t>MIF-2020-04-0001</t>
+  </si>
+  <si>
+    <t>WHP20-1000</t>
+  </si>
+  <si>
+    <t>PRO-PF 16-3 A</t>
+  </si>
+  <si>
+    <t>Adjusting Nut, PF 16-3A</t>
+  </si>
+  <si>
+    <t>pc/s</t>
+  </si>
+  <si>
+    <t>Progen Warehouse</t>
+  </si>
+  <si>
+    <t>Progen Consumables</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Progen Warehouse
 </t>
-  </si>
-  <si>
-    <t>40MVA Power Transformer Secondary Bus Framing/Support</t>
-  </si>
-  <si>
-    <t>1.5 MVA Station Transformer DG4 &amp; DG5 Generator Winding/VCB/MOCB/Cable Monitor</t>
-  </si>
-  <si>
-    <t>AUT-HEA_1002</t>
-  </si>
-  <si>
-    <t>Brake Shoe</t>
-  </si>
-  <si>
-    <t>set/s</t>
-  </si>
-  <si>
-    <t>7RJ Brothers Sand &amp; Gravel &amp; Gen. Mdse.</t>
   </si>
   <si>
     <t xml:space="preserve">Prepared By: </t>
@@ -267,18 +273,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="4" fillId="0" borderId="0" applyFont="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="0">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="0">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
+    <xf xfId="0" fontId="0" numFmtId="4" fillId="0" borderId="1" applyFont="0" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="2" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="0">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
@@ -334,7 +346,7 @@
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="1152525" cy="333375"/>
+    <xdr:ext cx="1104900" cy="333375"/>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="1" name="Sample image" descr="Sample image"/>
@@ -650,7 +662,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:AB18"/>
+  <dimension ref="A1:AF17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="O2" sqref="O2"/>
@@ -658,63 +670,67 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" spans="1:28">
-      <c r="A1" s="11"/>
-      <c r="B1" s="12"/>
-      <c r="C1" s="11" t="s">
+    <row r="1" spans="1:32">
+      <c r="A1" s="13"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="12"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5"/>
-      <c r="O1" s="5"/>
-      <c r="P1" s="5"/>
-      <c r="Q1" s="5"/>
-      <c r="R1" s="5"/>
-      <c r="S1" s="5"/>
-      <c r="T1" s="5"/>
-      <c r="U1" s="5"/>
-      <c r="V1" s="5"/>
-      <c r="W1" s="5"/>
-      <c r="X1" s="5"/>
-      <c r="Y1" s="5"/>
-      <c r="Z1" s="5"/>
-      <c r="AA1" s="5"/>
-      <c r="AB1" s="8"/>
-    </row>
-    <row r="2" spans="1:28">
-      <c r="A2" s="6"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
+      <c r="P1" s="7"/>
+      <c r="Q1" s="7"/>
+      <c r="R1" s="7"/>
+      <c r="S1" s="7"/>
+      <c r="T1" s="7"/>
+      <c r="U1" s="7"/>
+      <c r="V1" s="7"/>
+      <c r="W1" s="7"/>
+      <c r="X1" s="7"/>
+      <c r="Y1" s="7"/>
+      <c r="Z1" s="7"/>
+      <c r="AA1" s="7"/>
+      <c r="AB1" s="7"/>
+      <c r="AC1" s="7"/>
+      <c r="AD1" s="7"/>
+      <c r="AE1" s="7"/>
+      <c r="AF1" s="10"/>
+    </row>
+    <row r="2" spans="1:32">
+      <c r="A2" s="8"/>
       <c r="B2"/>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="8" t="s">
         <v>1</v>
       </c>
       <c r="D2"/>
       <c r="E2"/>
       <c r="F2"/>
       <c r="G2"/>
-      <c r="H2" s="14"/>
+      <c r="H2" s="16"/>
       <c r="I2"/>
       <c r="J2"/>
       <c r="K2"/>
       <c r="L2"/>
       <c r="M2"/>
       <c r="N2"/>
-      <c r="O2" s="15" t="s">
+      <c r="O2" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="P2" s="1"/>
-      <c r="Q2" s="1"/>
-      <c r="R2" s="1"/>
-      <c r="S2" s="1"/>
-      <c r="T2" s="1"/>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="3"/>
+      <c r="R2" s="3"/>
+      <c r="S2" s="3"/>
+      <c r="T2" s="3"/>
       <c r="U2"/>
       <c r="V2"/>
       <c r="W2"/>
@@ -722,343 +738,336 @@
       <c r="Y2"/>
       <c r="Z2"/>
       <c r="AA2"/>
-      <c r="AB2" s="9"/>
-    </row>
-    <row r="3" spans="1:28">
-      <c r="A3" s="7"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="7" t="s">
+      <c r="AB2"/>
+      <c r="AC2"/>
+      <c r="AD2"/>
+      <c r="AE2"/>
+      <c r="AF2" s="11"/>
+    </row>
+    <row r="3" spans="1:32">
+      <c r="A3" s="9"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4"/>
-      <c r="L3" s="4"/>
-      <c r="M3" s="4"/>
-      <c r="N3" s="4"/>
-      <c r="O3" s="4"/>
-      <c r="P3" s="4"/>
-      <c r="Q3" s="4"/>
-      <c r="R3" s="4"/>
-      <c r="S3" s="4"/>
-      <c r="T3" s="4"/>
-      <c r="U3" s="4"/>
-      <c r="V3" s="4"/>
-      <c r="W3" s="4"/>
-      <c r="X3" s="4"/>
-      <c r="Y3" s="4"/>
-      <c r="Z3" s="4"/>
-      <c r="AA3" s="4"/>
-      <c r="AB3" s="10"/>
-    </row>
-    <row r="5" spans="1:28">
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="6"/>
+      <c r="M3" s="6"/>
+      <c r="N3" s="6"/>
+      <c r="O3" s="6"/>
+      <c r="P3" s="6"/>
+      <c r="Q3" s="6"/>
+      <c r="R3" s="6"/>
+      <c r="S3" s="6"/>
+      <c r="T3" s="6"/>
+      <c r="U3" s="6"/>
+      <c r="V3" s="6"/>
+      <c r="W3" s="6"/>
+      <c r="X3" s="6"/>
+      <c r="Y3" s="6"/>
+      <c r="Z3" s="6"/>
+      <c r="AA3" s="6"/>
+      <c r="AB3" s="6"/>
+      <c r="AC3" s="6"/>
+      <c r="AD3" s="6"/>
+      <c r="AE3" s="6"/>
+      <c r="AF3" s="12"/>
+    </row>
+    <row r="5" spans="1:32">
       <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="C5" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="4"/>
-      <c r="G5" s="13" t="s">
+      <c r="E5" s="6"/>
+      <c r="G5" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="4" t="s">
+      <c r="H5" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="I5" s="4"/>
-    </row>
-    <row r="7" spans="1:28">
+      <c r="I5" s="6"/>
+      <c r="Q5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="R5" s="1"/>
+      <c r="S5" s="1">
+        <v>0</v>
+      </c>
+      <c r="T5" s="1"/>
+      <c r="U5" s="1"/>
+      <c r="V5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="Z5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:32">
+      <c r="Q6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="R6" s="1"/>
+      <c r="S6" s="1">
+        <v>0</v>
+      </c>
+      <c r="T6" s="1"/>
+      <c r="U6" s="1"/>
+      <c r="V6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:32">
       <c r="A7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:28">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:32">
       <c r="A8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
+        <v>14</v>
+      </c>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
       <c r="F8" t="s">
-        <v>11</v>
-      </c>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
-      <c r="J8" s="4"/>
+        <v>15</v>
+      </c>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
       <c r="L8" t="s">
-        <v>12</v>
-      </c>
-      <c r="M8" s="4"/>
-      <c r="N8" s="4"/>
-      <c r="O8" s="4"/>
-    </row>
-    <row r="10" spans="1:28">
-      <c r="A10" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2" t="s">
+      <c r="M8" s="6"/>
+      <c r="N8" s="6"/>
+      <c r="O8" s="6"/>
+    </row>
+    <row r="10" spans="1:32">
+      <c r="A10" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
-      <c r="L10" s="2" t="s">
+      <c r="B10" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="M10" s="2" t="s">
+      <c r="C10" s="5"/>
+      <c r="D10" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="N10" s="2"/>
-      <c r="O10" s="2" t="s">
+      <c r="E10" s="5"/>
+      <c r="F10" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="P10" s="2"/>
-      <c r="Q10" s="2"/>
-      <c r="R10" s="2" t="s">
+      <c r="G10" s="5"/>
+      <c r="H10" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="S10" s="2"/>
-      <c r="T10" s="2"/>
-      <c r="U10" s="2" t="s">
+      <c r="I10" s="5"/>
+      <c r="J10" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="V10" s="2"/>
-      <c r="W10" s="2"/>
-      <c r="X10" s="2" t="s">
+      <c r="K10" s="5"/>
+      <c r="L10" s="5"/>
+      <c r="M10" s="5"/>
+      <c r="N10" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="Y10" s="2"/>
-      <c r="Z10" s="2"/>
-      <c r="AA10" s="2" t="s">
+      <c r="O10" s="5"/>
+      <c r="P10" s="5"/>
+      <c r="Q10" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="AB10" s="3"/>
-    </row>
-    <row r="11" spans="1:28">
-      <c r="A11" s="3">
+      <c r="R10" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="S10" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="T10" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="U10" s="5"/>
+      <c r="V10" s="5"/>
+      <c r="W10" s="5"/>
+      <c r="X10" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y10" s="5"/>
+      <c r="Z10" s="5"/>
+      <c r="AA10" s="5"/>
+      <c r="AB10" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="AC10" s="5"/>
+      <c r="AD10" s="5"/>
+      <c r="AE10" s="5"/>
+      <c r="AF10" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:32">
+      <c r="A11" s="2">
         <v>1</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3" t="s">
+      <c r="B11" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="5"/>
+      <c r="D11" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="4">
         <v>26</v>
       </c>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="3"/>
-      <c r="L11" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="M11" s="2">
-        <v>12</v>
-      </c>
-      <c r="N11" s="2"/>
-      <c r="O11" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="P11" s="3"/>
-      <c r="Q11" s="3"/>
-      <c r="R11" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="S11" s="3"/>
-      <c r="T11" s="3"/>
-      <c r="U11" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="V11" s="3"/>
-      <c r="W11" s="3"/>
-      <c r="X11" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="Y11" s="3"/>
-      <c r="Z11" s="3"/>
-      <c r="AA11" s="3"/>
-      <c r="AB11" s="3"/>
-    </row>
-    <row r="12" spans="1:28">
-      <c r="A12" s="3">
-        <v>2</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>25</v>
-      </c>
+      <c r="O11" s="4"/>
+      <c r="P11" s="4"/>
+      <c r="Q11" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="R11" s="4">
+        <v>0</v>
+      </c>
+      <c r="S11" s="5">
+        <v>0</v>
+      </c>
+      <c r="T11" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="U11" s="2"/>
+      <c r="V11" s="2"/>
+      <c r="W11" s="2"/>
+      <c r="X11" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y11" s="2"/>
+      <c r="Z11" s="2"/>
+      <c r="AA11" s="2"/>
+      <c r="AB11" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC11" s="2"/>
+      <c r="AD11" s="2"/>
+      <c r="AE11" s="2"/>
+      <c r="AF11" s="2"/>
+    </row>
+    <row r="12" spans="1:32">
+      <c r="B12" s="3"/>
       <c r="C12" s="3"/>
-      <c r="D12" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="3"/>
-      <c r="L12" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="M12" s="2">
-        <v>7</v>
-      </c>
-      <c r="N12" s="2"/>
-      <c r="O12" s="3" t="s">
-        <v>37</v>
-      </c>
+      <c r="D12"/>
+      <c r="E12"/>
+      <c r="F12"/>
+      <c r="G12"/>
+      <c r="H12"/>
+      <c r="I12"/>
+      <c r="J12"/>
+      <c r="K12"/>
+      <c r="L12"/>
+      <c r="M12"/>
+      <c r="N12" s="3"/>
+      <c r="O12" s="3"/>
       <c r="P12" s="3"/>
       <c r="Q12" s="3"/>
-      <c r="R12" s="3" t="s">
-        <v>31</v>
-      </c>
+      <c r="R12" s="3"/>
       <c r="S12" s="3"/>
-      <c r="T12" s="3"/>
-      <c r="U12" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="V12" s="3"/>
-      <c r="W12" s="3"/>
-      <c r="X12" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="Y12" s="3"/>
-      <c r="Z12" s="3"/>
-      <c r="AA12" s="3"/>
-      <c r="AB12" s="3"/>
-    </row>
-    <row r="13" spans="1:28">
-      <c r="B13"/>
-      <c r="C13"/>
-      <c r="D13"/>
-      <c r="E13"/>
-      <c r="F13"/>
-      <c r="G13"/>
-      <c r="H13"/>
-      <c r="I13"/>
-      <c r="J13"/>
-      <c r="K13"/>
-      <c r="L13" s="1"/>
-      <c r="M13" s="1"/>
-      <c r="N13" s="1"/>
-      <c r="O13"/>
-      <c r="P13"/>
-      <c r="Q13"/>
-      <c r="R13"/>
-      <c r="S13"/>
-      <c r="T13"/>
-      <c r="U13"/>
-      <c r="V13"/>
-      <c r="W13"/>
-      <c r="X13"/>
-      <c r="Y13"/>
-      <c r="Z13"/>
-      <c r="AA13"/>
-      <c r="AB13"/>
-    </row>
-    <row r="15" spans="1:28">
-      <c r="A15" t="s">
-        <v>38</v>
-      </c>
-      <c r="D15" t="s">
-        <v>39</v>
-      </c>
-      <c r="G15" t="s">
+      <c r="T12"/>
+      <c r="U12"/>
+      <c r="V12"/>
+      <c r="W12"/>
+      <c r="X12"/>
+      <c r="Y12"/>
+      <c r="Z12"/>
+      <c r="AA12"/>
+      <c r="AB12"/>
+      <c r="AC12"/>
+      <c r="AD12"/>
+      <c r="AE12"/>
+    </row>
+    <row r="14" spans="1:32">
+      <c r="A14" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="18" spans="1:28">
-      <c r="A18" t="s">
+      <c r="D14" t="s">
         <v>41</v>
       </c>
-      <c r="D18" t="s">
+      <c r="G14" t="s">
         <v>42</v>
       </c>
-      <c r="G18" t="s">
+    </row>
+    <row r="17" spans="1:32">
+      <c r="A17" t="s">
         <v>43</v>
+      </c>
+      <c r="D17" t="s">
+        <v>44</v>
+      </c>
+      <c r="G17" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection sheet="true" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
   <protectedRanges>
-    <protectedRange name="p1271e4ddd8b869e97602621c363a49f7" sqref="A11:AA11" password="C724"/>
-    <protectedRange name="pf6115c49b9bde900a9d95288048e32e4" sqref="A12:AA12" password="C724"/>
-    <protectedRange name="p6609b117f3410da1c99f884a2864736d" sqref="A15:AC15" password="C724"/>
-    <protectedRange name="pa5ff55bbf8d64ae537a78f01c5d0c668" sqref="A17:AC17" password="C724"/>
+    <protectedRange name="p7da39a9eb4691c391f85ef17c1a72749" sqref="A11:AF11" password="C724"/>
+    <protectedRange name="pb92778bd78a4353a4ab9294156805e41" sqref="A14:AC14" password="C724"/>
+    <protectedRange name="p3a834472df22454fed33e8b780f2ec25" sqref="A16:AC16" password="C724"/>
   </protectedRanges>
   <mergeCells>
+    <mergeCell ref="B11:C11"/>
     <mergeCell ref="B12:C12"/>
     <mergeCell ref="D11:E11"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="F11:G11"/>
     <mergeCell ref="F12:G12"/>
-    <mergeCell ref="H11:K11"/>
-    <mergeCell ref="H12:K12"/>
-    <mergeCell ref="M11:N11"/>
-    <mergeCell ref="M12:N12"/>
-    <mergeCell ref="O11:Q11"/>
-    <mergeCell ref="O12:Q12"/>
-    <mergeCell ref="R11:T11"/>
-    <mergeCell ref="R12:T12"/>
-    <mergeCell ref="U11:W11"/>
-    <mergeCell ref="U12:W12"/>
-    <mergeCell ref="X11:Z11"/>
-    <mergeCell ref="X12:Z12"/>
-    <mergeCell ref="AA11:AB11"/>
-    <mergeCell ref="AA12:AB12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="H13:K13"/>
-    <mergeCell ref="M13:N13"/>
-    <mergeCell ref="O13:Q13"/>
-    <mergeCell ref="R13:T13"/>
-    <mergeCell ref="U13:W13"/>
-    <mergeCell ref="X13:Z13"/>
-    <mergeCell ref="AA13:AB13"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="J11:M11"/>
+    <mergeCell ref="J12:M12"/>
+    <mergeCell ref="N11:P11"/>
+    <mergeCell ref="N12:P12"/>
+    <mergeCell ref="T11:W11"/>
+    <mergeCell ref="T12:W12"/>
+    <mergeCell ref="X11:AA11"/>
+    <mergeCell ref="X12:AA12"/>
+    <mergeCell ref="AB11:AE11"/>
+    <mergeCell ref="AB12:AE12"/>
     <mergeCell ref="O2:T2"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="D10:E10"/>
     <mergeCell ref="F10:G10"/>
-    <mergeCell ref="H10:K10"/>
-    <mergeCell ref="M10:N10"/>
-    <mergeCell ref="O10:Q10"/>
-    <mergeCell ref="R10:T10"/>
-    <mergeCell ref="U10:W10"/>
-    <mergeCell ref="X10:Z10"/>
-    <mergeCell ref="AA10:AB10"/>
-    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="J10:M10"/>
+    <mergeCell ref="N10:P10"/>
+    <mergeCell ref="T10:W10"/>
+    <mergeCell ref="X10:AA10"/>
+    <mergeCell ref="AB10:AE10"/>
   </mergeCells>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add Dr No. in Receive and Issue Report and Exported file
</commit_message>
<xml_diff>
--- a/Issued Report.xlsx
+++ b/Issued Report.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="100">
   <si>
     <t>PROGEN DIESEL TECH</t>
   </si>
@@ -35,15 +35,15 @@
     <t>TO</t>
   </si>
   <si>
+    <t>2020-02-01</t>
+  </si>
+  <si>
+    <t>FROM</t>
+  </si>
+  <si>
     <t>2020-03-01</t>
   </si>
   <si>
-    <t>FROM</t>
-  </si>
-  <si>
-    <t>2020-04-27</t>
-  </si>
-  <si>
     <t xml:space="preserve">Total Cost w/ PR: </t>
   </si>
   <si>
@@ -74,6 +74,9 @@
     <t>Issue Date</t>
   </si>
   <si>
+    <t>DR No.</t>
+  </si>
+  <si>
     <t>MIF No.</t>
   </si>
   <si>
@@ -110,32 +113,191 @@
     <t>Frequency</t>
   </si>
   <si>
-    <t>2020-04-22</t>
-  </si>
-  <si>
-    <t>MIF-2020-04-0001</t>
-  </si>
-  <si>
-    <t>WHP20-1000</t>
-  </si>
-  <si>
-    <t>PRO-PF 16-3 A</t>
-  </si>
-  <si>
-    <t>Adjusting Nut, PF 16-3A</t>
-  </si>
-  <si>
-    <t>pc/s</t>
+    <t>2020-02-24</t>
+  </si>
+  <si>
+    <t>MIF-2020-02-0018</t>
+  </si>
+  <si>
+    <t>PROGEN-006-2019</t>
+  </si>
+  <si>
+    <t>CON-FUE_1001</t>
+  </si>
+  <si>
+    <t>Diesel, Fuel-Save</t>
+  </si>
+  <si>
+    <t>ltr/s</t>
+  </si>
+  <si>
+    <t>Progen CV</t>
+  </si>
+  <si>
+    <t>Dismantling, cleaning, inspection, crack testing, measurement &amp; evaluation, reassembling &amp; preservation.</t>
+  </si>
+  <si>
+    <t>DG4 (CV Area) Main Engine Parts &amp; Components</t>
+  </si>
+  <si>
+    <t>2020-02-22</t>
+  </si>
+  <si>
+    <t>MIF-2020-02-0002</t>
+  </si>
+  <si>
+    <t>PROGEN-008-2019</t>
+  </si>
+  <si>
+    <t>CON-HOU_1001</t>
+  </si>
+  <si>
+    <t>Rags, Cotton</t>
+  </si>
+  <si>
+    <t>kg/s</t>
   </si>
   <si>
     <t>Progen Warehouse</t>
   </si>
   <si>
-    <t>Progen Consumables</t>
+    <t>Consumables / Cleaning &amp; Preservation of Spare parts</t>
   </si>
   <si>
     <t xml:space="preserve">Progen Warehouse
 </t>
+  </si>
+  <si>
+    <t>MIF-2020-02-0006</t>
+  </si>
+  <si>
+    <t>PROGEN-002-2020</t>
+  </si>
+  <si>
+    <t>CON-CON_1004</t>
+  </si>
+  <si>
+    <t>Paint Brush 2"</t>
+  </si>
+  <si>
+    <t>pc/s</t>
+  </si>
+  <si>
+    <t>Progen Consumables</t>
+  </si>
+  <si>
+    <t>DG2 Main Engine Frame Cleaning and Preserving</t>
+  </si>
+  <si>
+    <t>MIF-2020-02-0007</t>
+  </si>
+  <si>
+    <t>PROGEN-002-2019</t>
+  </si>
+  <si>
+    <t>DG1 (CV Area) Main Engine Parts &amp; Components.</t>
+  </si>
+  <si>
+    <t>MIF-2020-02-0009</t>
+  </si>
+  <si>
+    <t>PROGEN-011-2019</t>
+  </si>
+  <si>
+    <t>CON-CON_1019</t>
+  </si>
+  <si>
+    <t>Thinner; Lacquer, Brand: CES/ML</t>
+  </si>
+  <si>
+    <t>gal/s</t>
+  </si>
+  <si>
+    <t>Equipment @ CV yard</t>
+  </si>
+  <si>
+    <t>MIF-2020-02-0017</t>
+  </si>
+  <si>
+    <t>2020-02-21</t>
+  </si>
+  <si>
+    <t>2019-006</t>
+  </si>
+  <si>
+    <t>MIF-2020-02-0013</t>
+  </si>
+  <si>
+    <t>PROGEN-267-2019</t>
+  </si>
+  <si>
+    <t>CON-CHE_1001</t>
+  </si>
+  <si>
+    <t>Vappro 868 VCI Corrosion Inbitor Wax Coating (4 liters/gallon)</t>
+  </si>
+  <si>
+    <t>2020-02-17</t>
+  </si>
+  <si>
+    <t>MIF-2020-02-0001</t>
+  </si>
+  <si>
+    <t>MIF-2020-02-0014</t>
+  </si>
+  <si>
+    <t>CON-FUE_1002</t>
+  </si>
+  <si>
+    <t>Penetrating Oil Multi Use, WD40</t>
+  </si>
+  <si>
+    <t>can/s</t>
+  </si>
+  <si>
+    <t>MIF-2020-02-0015</t>
+  </si>
+  <si>
+    <t>CON-HOU_1002</t>
+  </si>
+  <si>
+    <t>Broom (Paypay)</t>
+  </si>
+  <si>
+    <t>CON-HOU_1012</t>
+  </si>
+  <si>
+    <t>Broom Stick</t>
+  </si>
+  <si>
+    <t>MIF-2020-02-0016</t>
+  </si>
+  <si>
+    <t>CON-HOU_1013</t>
+  </si>
+  <si>
+    <t>Plastic; Resealable, #5, (1 pack=100 pcs)</t>
+  </si>
+  <si>
+    <t>pack/s</t>
+  </si>
+  <si>
+    <t>CON-HOU_1014</t>
+  </si>
+  <si>
+    <t>Plastic; Resealable, #7, (1 pack=100 pcs)</t>
+  </si>
+  <si>
+    <t>2020-02-06</t>
+  </si>
+  <si>
+    <t>MIF-2020-02-0004</t>
+  </si>
+  <si>
+    <t>CON-CON_1003</t>
+  </si>
+  <si>
+    <t>Sand Paper, G120</t>
   </si>
   <si>
     <t xml:space="preserve">Prepared By: </t>
@@ -286,10 +448,10 @@
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="0" numFmtId="4" fillId="0" borderId="1" applyFont="0" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" fontId="0" numFmtId="4" fillId="0" borderId="1" applyFont="0" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="2" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="0">
@@ -662,7 +824,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:AF17"/>
+  <dimension ref="A1:AF30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="O2" sqref="O2"/>
@@ -803,7 +965,7 @@
       </c>
       <c r="R5" s="1"/>
       <c r="S5" s="1">
-        <v>0</v>
+        <v>27888.7</v>
       </c>
       <c r="T5" s="1"/>
       <c r="U5" s="1"/>
@@ -828,7 +990,7 @@
         <v>12</v>
       </c>
       <c r="Z6">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:32">
@@ -857,121 +1019,125 @@
       <c r="O8" s="6"/>
     </row>
     <row r="10" spans="1:32">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5" t="s">
+      <c r="C10" s="4"/>
+      <c r="D10" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5" t="s">
+      <c r="E10" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5" t="s">
+      <c r="F10" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="I10" s="5"/>
-      <c r="J10" s="5" t="s">
+      <c r="G10" s="4"/>
+      <c r="H10" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="K10" s="5"/>
-      <c r="L10" s="5"/>
-      <c r="M10" s="5"/>
-      <c r="N10" s="5" t="s">
+      <c r="I10" s="4"/>
+      <c r="J10" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="O10" s="5"/>
-      <c r="P10" s="5"/>
-      <c r="Q10" s="5" t="s">
+      <c r="K10" s="4"/>
+      <c r="L10" s="4"/>
+      <c r="M10" s="4"/>
+      <c r="N10" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="R10" s="5" t="s">
+      <c r="O10" s="4"/>
+      <c r="P10" s="4"/>
+      <c r="Q10" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="S10" s="5" t="s">
+      <c r="R10" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="T10" s="5" t="s">
+      <c r="S10" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="U10" s="5"/>
-      <c r="V10" s="5"/>
-      <c r="W10" s="5"/>
-      <c r="X10" s="5" t="s">
+      <c r="T10" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="Y10" s="5"/>
-      <c r="Z10" s="5"/>
-      <c r="AA10" s="5"/>
-      <c r="AB10" s="5" t="s">
+      <c r="U10" s="4"/>
+      <c r="V10" s="4"/>
+      <c r="W10" s="4"/>
+      <c r="X10" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="AC10" s="5"/>
-      <c r="AD10" s="5"/>
-      <c r="AE10" s="5"/>
-      <c r="AF10" s="5" t="s">
+      <c r="Y10" s="4"/>
+      <c r="Z10" s="4"/>
+      <c r="AA10" s="4"/>
+      <c r="AB10" s="4" t="s">
         <v>30</v>
+      </c>
+      <c r="AC10" s="4"/>
+      <c r="AD10" s="4"/>
+      <c r="AE10" s="4"/>
+      <c r="AF10" s="4" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:32">
       <c r="A11" s="2">
         <v>1</v>
       </c>
-      <c r="B11" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C11" s="5"/>
-      <c r="D11" s="2" t="s">
+      <c r="B11" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="E11" s="2"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="2">
+        <v>77</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="F11" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G11" s="2"/>
       <c r="H11" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="I11" s="2"/>
       <c r="J11" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="K11" s="2"/>
       <c r="L11" s="2"/>
       <c r="M11" s="2"/>
-      <c r="N11" s="4">
-        <v>26</v>
-      </c>
-      <c r="O11" s="4"/>
-      <c r="P11" s="4"/>
-      <c r="Q11" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="R11" s="4">
-        <v>0</v>
-      </c>
-      <c r="S11" s="5">
-        <v>0</v>
+      <c r="N11" s="5">
+        <v>11</v>
+      </c>
+      <c r="O11" s="5"/>
+      <c r="P11" s="5"/>
+      <c r="Q11" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="R11" s="5">
+        <v>37.3</v>
+      </c>
+      <c r="S11" s="4">
+        <v>410.3</v>
       </c>
       <c r="T11" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="U11" s="2"/>
       <c r="V11" s="2"/>
       <c r="W11" s="2"/>
       <c r="X11" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="Y11" s="2"/>
       <c r="Z11" s="2"/>
       <c r="AA11" s="2"/>
       <c r="AB11" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AC11" s="2"/>
       <c r="AD11" s="2"/>
@@ -979,71 +1145,886 @@
       <c r="AF11" s="2"/>
     </row>
     <row r="12" spans="1:32">
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12"/>
-      <c r="E12"/>
-      <c r="F12"/>
-      <c r="G12"/>
-      <c r="H12"/>
-      <c r="I12"/>
-      <c r="J12"/>
-      <c r="K12"/>
-      <c r="L12"/>
-      <c r="M12"/>
-      <c r="N12" s="3"/>
-      <c r="O12" s="3"/>
-      <c r="P12" s="3"/>
-      <c r="Q12" s="3"/>
-      <c r="R12" s="3"/>
-      <c r="S12" s="3"/>
-      <c r="T12"/>
-      <c r="U12"/>
-      <c r="V12"/>
-      <c r="W12"/>
-      <c r="X12"/>
-      <c r="Y12"/>
-      <c r="Z12"/>
-      <c r="AA12"/>
-      <c r="AB12"/>
-      <c r="AC12"/>
-      <c r="AD12"/>
-      <c r="AE12"/>
+      <c r="A12" s="2">
+        <v>2</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" s="4"/>
+      <c r="D12" s="2">
+        <v>55</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
+      <c r="N12" s="5">
+        <v>5</v>
+      </c>
+      <c r="O12" s="5"/>
+      <c r="P12" s="5"/>
+      <c r="Q12" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="R12" s="5">
+        <v>50</v>
+      </c>
+      <c r="S12" s="4">
+        <v>250</v>
+      </c>
+      <c r="T12" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="U12" s="2"/>
+      <c r="V12" s="2"/>
+      <c r="W12" s="2"/>
+      <c r="X12" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y12" s="2"/>
+      <c r="Z12" s="2"/>
+      <c r="AA12" s="2"/>
+      <c r="AB12" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="AC12" s="2"/>
+      <c r="AD12" s="2"/>
+      <c r="AE12" s="2"/>
+      <c r="AF12" s="2"/>
+    </row>
+    <row r="13" spans="1:32">
+      <c r="A13" s="2">
+        <v>3</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C13" s="4"/>
+      <c r="D13" s="2">
+        <v>67</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+      <c r="N13" s="5">
+        <v>5</v>
+      </c>
+      <c r="O13" s="5"/>
+      <c r="P13" s="5"/>
+      <c r="Q13" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="R13" s="5">
+        <v>12.5</v>
+      </c>
+      <c r="S13" s="4">
+        <v>62.5</v>
+      </c>
+      <c r="T13" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="U13" s="2"/>
+      <c r="V13" s="2"/>
+      <c r="W13" s="2"/>
+      <c r="X13" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="Y13" s="2"/>
+      <c r="Z13" s="2"/>
+      <c r="AA13" s="2"/>
+      <c r="AB13" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AC13" s="2"/>
+      <c r="AD13" s="2"/>
+      <c r="AE13" s="2"/>
+      <c r="AF13" s="2"/>
     </row>
     <row r="14" spans="1:32">
-      <c r="A14" t="s">
+      <c r="A14" s="2">
+        <v>4</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C14" s="4"/>
+      <c r="D14" s="2">
         <v>40</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
+      <c r="M14" s="2"/>
+      <c r="N14" s="5">
+        <v>5</v>
+      </c>
+      <c r="O14" s="5"/>
+      <c r="P14" s="5"/>
+      <c r="Q14" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="R14" s="5">
+        <v>12.5</v>
+      </c>
+      <c r="S14" s="4">
+        <v>62.5</v>
+      </c>
+      <c r="T14" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="U14" s="2"/>
+      <c r="V14" s="2"/>
+      <c r="W14" s="2"/>
+      <c r="X14" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y14" s="2"/>
+      <c r="Z14" s="2"/>
+      <c r="AA14" s="2"/>
+      <c r="AB14" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC14" s="2"/>
+      <c r="AD14" s="2"/>
+      <c r="AE14" s="2"/>
+      <c r="AF14" s="2"/>
+    </row>
+    <row r="15" spans="1:32">
+      <c r="A15" s="2">
+        <v>5</v>
+      </c>
+      <c r="B15" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="G14" t="s">
-        <v>42</v>
-      </c>
+      <c r="C15" s="4"/>
+      <c r="D15" s="2">
+        <v>70</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
+      <c r="M15" s="2"/>
+      <c r="N15" s="5">
+        <v>2</v>
+      </c>
+      <c r="O15" s="5"/>
+      <c r="P15" s="5"/>
+      <c r="Q15" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="R15" s="5">
+        <v>220</v>
+      </c>
+      <c r="S15" s="4">
+        <v>440</v>
+      </c>
+      <c r="T15" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="U15" s="2"/>
+      <c r="V15" s="2"/>
+      <c r="W15" s="2"/>
+      <c r="X15" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="Y15" s="2"/>
+      <c r="Z15" s="2"/>
+      <c r="AA15" s="2"/>
+      <c r="AB15" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="AC15" s="2"/>
+      <c r="AD15" s="2"/>
+      <c r="AE15" s="2"/>
+      <c r="AF15" s="2"/>
+    </row>
+    <row r="16" spans="1:32">
+      <c r="A16" s="2">
+        <v>6</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16" s="4"/>
+      <c r="D16" s="2">
+        <v>76</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="K16" s="2"/>
+      <c r="L16" s="2"/>
+      <c r="M16" s="2"/>
+      <c r="N16" s="5">
+        <v>8</v>
+      </c>
+      <c r="O16" s="5"/>
+      <c r="P16" s="5"/>
+      <c r="Q16" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="R16" s="5">
+        <v>37.3</v>
+      </c>
+      <c r="S16" s="4">
+        <v>298.4</v>
+      </c>
+      <c r="T16" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="U16" s="2"/>
+      <c r="V16" s="2"/>
+      <c r="W16" s="2"/>
+      <c r="X16" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y16" s="2"/>
+      <c r="Z16" s="2"/>
+      <c r="AA16" s="2"/>
+      <c r="AB16" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC16" s="2"/>
+      <c r="AD16" s="2"/>
+      <c r="AE16" s="2"/>
+      <c r="AF16" s="2"/>
     </row>
     <row r="17" spans="1:32">
-      <c r="A17" t="s">
+      <c r="A17" s="2">
+        <v>7</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C17" s="4"/>
+      <c r="D17" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="K17" s="2"/>
+      <c r="L17" s="2"/>
+      <c r="M17" s="2"/>
+      <c r="N17" s="5">
+        <v>2</v>
+      </c>
+      <c r="O17" s="5"/>
+      <c r="P17" s="5"/>
+      <c r="Q17" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="R17" s="5">
+        <v>12320</v>
+      </c>
+      <c r="S17" s="4">
+        <v>24640</v>
+      </c>
+      <c r="T17" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="U17" s="2"/>
+      <c r="V17" s="2"/>
+      <c r="W17" s="2"/>
+      <c r="X17" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="Y17" s="2"/>
+      <c r="Z17" s="2"/>
+      <c r="AA17" s="2"/>
+      <c r="AB17" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="AC17" s="2"/>
+      <c r="AD17" s="2"/>
+      <c r="AE17" s="2"/>
+      <c r="AF17" s="2"/>
+    </row>
+    <row r="18" spans="1:32">
+      <c r="A18" s="2">
+        <v>8</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C18" s="4"/>
+      <c r="D18" s="2">
+        <v>64</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="K18" s="2"/>
+      <c r="L18" s="2"/>
+      <c r="M18" s="2"/>
+      <c r="N18" s="5">
+        <v>5</v>
+      </c>
+      <c r="O18" s="5"/>
+      <c r="P18" s="5"/>
+      <c r="Q18" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="R18" s="5">
+        <v>50</v>
+      </c>
+      <c r="S18" s="4">
+        <v>250</v>
+      </c>
+      <c r="T18" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="U18" s="2"/>
+      <c r="V18" s="2"/>
+      <c r="W18" s="2"/>
+      <c r="X18" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="Y18" s="2"/>
+      <c r="Z18" s="2"/>
+      <c r="AA18" s="2"/>
+      <c r="AB18" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AC18" s="2"/>
+      <c r="AD18" s="2"/>
+      <c r="AE18" s="2"/>
+      <c r="AF18" s="2"/>
+    </row>
+    <row r="19" spans="1:32">
+      <c r="A19" s="2">
+        <v>9</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C19" s="4"/>
+      <c r="D19" s="2">
+        <v>66</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="K19" s="2"/>
+      <c r="L19" s="2"/>
+      <c r="M19" s="2"/>
+      <c r="N19" s="5">
+        <v>3</v>
+      </c>
+      <c r="O19" s="5"/>
+      <c r="P19" s="5"/>
+      <c r="Q19" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="R19" s="5">
+        <v>210</v>
+      </c>
+      <c r="S19" s="4">
+        <v>630</v>
+      </c>
+      <c r="T19" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="U19" s="2"/>
+      <c r="V19" s="2"/>
+      <c r="W19" s="2"/>
+      <c r="X19" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="Y19" s="2"/>
+      <c r="Z19" s="2"/>
+      <c r="AA19" s="2"/>
+      <c r="AB19" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AC19" s="2"/>
+      <c r="AD19" s="2"/>
+      <c r="AE19" s="2"/>
+      <c r="AF19" s="2"/>
+    </row>
+    <row r="20" spans="1:32">
+      <c r="A20" s="2">
+        <v>10</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C20" s="4"/>
+      <c r="D20" s="2">
+        <v>73</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="K20" s="2"/>
+      <c r="L20" s="2"/>
+      <c r="M20" s="2"/>
+      <c r="N20" s="5">
+        <v>2</v>
+      </c>
+      <c r="O20" s="5"/>
+      <c r="P20" s="5"/>
+      <c r="Q20" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="R20" s="5">
+        <v>45</v>
+      </c>
+      <c r="S20" s="4">
+        <v>90</v>
+      </c>
+      <c r="T20" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="U20" s="2"/>
+      <c r="V20" s="2"/>
+      <c r="W20" s="2"/>
+      <c r="X20" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="Y20" s="2"/>
+      <c r="Z20" s="2"/>
+      <c r="AA20" s="2"/>
+      <c r="AB20" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="AC20" s="2"/>
+      <c r="AD20" s="2"/>
+      <c r="AE20" s="2"/>
+      <c r="AF20" s="2"/>
+    </row>
+    <row r="21" spans="1:32">
+      <c r="A21" s="2">
+        <v>11</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C21" s="4"/>
+      <c r="D21" s="2">
+        <v>73</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="I21" s="2"/>
+      <c r="J21" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="K21" s="2"/>
+      <c r="L21" s="2"/>
+      <c r="M21" s="2"/>
+      <c r="N21" s="5">
+        <v>2</v>
+      </c>
+      <c r="O21" s="5"/>
+      <c r="P21" s="5"/>
+      <c r="Q21" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="R21" s="5">
+        <v>30</v>
+      </c>
+      <c r="S21" s="4">
+        <v>60</v>
+      </c>
+      <c r="T21" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="U21" s="2"/>
+      <c r="V21" s="2"/>
+      <c r="W21" s="2"/>
+      <c r="X21" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="Y21" s="2"/>
+      <c r="Z21" s="2"/>
+      <c r="AA21" s="2"/>
+      <c r="AB21" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="AC21" s="2"/>
+      <c r="AD21" s="2"/>
+      <c r="AE21" s="2"/>
+      <c r="AF21" s="2"/>
+    </row>
+    <row r="22" spans="1:32">
+      <c r="A22" s="2">
+        <v>12</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C22" s="4"/>
+      <c r="D22" s="2">
+        <v>75</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="F22" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D17" t="s">
-        <v>44</v>
-      </c>
-      <c r="G17" t="s">
-        <v>45</v>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="I22" s="2"/>
+      <c r="J22" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="K22" s="2"/>
+      <c r="L22" s="2"/>
+      <c r="M22" s="2"/>
+      <c r="N22" s="5">
+        <v>1</v>
+      </c>
+      <c r="O22" s="5"/>
+      <c r="P22" s="5"/>
+      <c r="Q22" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="R22" s="5">
+        <v>70</v>
+      </c>
+      <c r="S22" s="4">
+        <v>70</v>
+      </c>
+      <c r="T22" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="U22" s="2"/>
+      <c r="V22" s="2"/>
+      <c r="W22" s="2"/>
+      <c r="X22" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y22" s="2"/>
+      <c r="Z22" s="2"/>
+      <c r="AA22" s="2"/>
+      <c r="AB22" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="AC22" s="2"/>
+      <c r="AD22" s="2"/>
+      <c r="AE22" s="2"/>
+      <c r="AF22" s="2"/>
+    </row>
+    <row r="23" spans="1:32">
+      <c r="A23" s="2">
+        <v>13</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C23" s="4"/>
+      <c r="D23" s="2">
+        <v>75</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="I23" s="2"/>
+      <c r="J23" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="K23" s="2"/>
+      <c r="L23" s="2"/>
+      <c r="M23" s="2"/>
+      <c r="N23" s="5">
+        <v>1</v>
+      </c>
+      <c r="O23" s="5"/>
+      <c r="P23" s="5"/>
+      <c r="Q23" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="R23" s="5">
+        <v>125</v>
+      </c>
+      <c r="S23" s="4">
+        <v>125</v>
+      </c>
+      <c r="T23" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="U23" s="2"/>
+      <c r="V23" s="2"/>
+      <c r="W23" s="2"/>
+      <c r="X23" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y23" s="2"/>
+      <c r="Z23" s="2"/>
+      <c r="AA23" s="2"/>
+      <c r="AB23" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="AC23" s="2"/>
+      <c r="AD23" s="2"/>
+      <c r="AE23" s="2"/>
+      <c r="AF23" s="2"/>
+    </row>
+    <row r="24" spans="1:32">
+      <c r="A24" s="2">
+        <v>14</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="C24" s="4"/>
+      <c r="D24" s="2">
+        <v>103</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="K24" s="2"/>
+      <c r="L24" s="2"/>
+      <c r="M24" s="2"/>
+      <c r="N24" s="5">
+        <v>50</v>
+      </c>
+      <c r="O24" s="5"/>
+      <c r="P24" s="5"/>
+      <c r="Q24" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="R24" s="5">
+        <v>10</v>
+      </c>
+      <c r="S24" s="4">
+        <v>500</v>
+      </c>
+      <c r="T24" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="U24" s="2"/>
+      <c r="V24" s="2"/>
+      <c r="W24" s="2"/>
+      <c r="X24" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y24" s="2"/>
+      <c r="Z24" s="2"/>
+      <c r="AA24" s="2"/>
+      <c r="AB24" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="AC24" s="2"/>
+      <c r="AD24" s="2"/>
+      <c r="AE24" s="2"/>
+      <c r="AF24" s="2"/>
+    </row>
+    <row r="25" spans="1:32">
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="F25"/>
+      <c r="G25"/>
+      <c r="H25"/>
+      <c r="I25"/>
+      <c r="J25"/>
+      <c r="K25"/>
+      <c r="L25"/>
+      <c r="M25"/>
+      <c r="N25" s="3"/>
+      <c r="O25" s="3"/>
+      <c r="P25" s="3"/>
+      <c r="Q25" s="3"/>
+      <c r="R25" s="3"/>
+      <c r="S25" s="3"/>
+      <c r="T25"/>
+      <c r="U25"/>
+      <c r="V25"/>
+      <c r="W25"/>
+      <c r="X25"/>
+      <c r="Y25"/>
+      <c r="Z25"/>
+      <c r="AA25"/>
+      <c r="AB25"/>
+      <c r="AC25"/>
+      <c r="AD25"/>
+      <c r="AE25"/>
+    </row>
+    <row r="27" spans="1:32">
+      <c r="A27" t="s">
+        <v>94</v>
+      </c>
+      <c r="D27" t="s">
+        <v>95</v>
+      </c>
+      <c r="G27" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="30" spans="1:32">
+      <c r="A30" t="s">
+        <v>97</v>
+      </c>
+      <c r="D30" t="s">
+        <v>98</v>
+      </c>
+      <c r="G30" t="s">
+        <v>99</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection sheet="true" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
   <protectedRanges>
     <protectedRange name="p7da39a9eb4691c391f85ef17c1a72749" sqref="A11:AF11" password="C724"/>
-    <protectedRange name="pb92778bd78a4353a4ab9294156805e41" sqref="A14:AC14" password="C724"/>
-    <protectedRange name="p3a834472df22454fed33e8b780f2ec25" sqref="A16:AC16" password="C724"/>
+    <protectedRange name="pfdf46eb298a00ec7897a94c36413667e" sqref="A12:AF12" password="C724"/>
+    <protectedRange name="p2db611be83b0829e14f5d0ca58f9df93" sqref="A13:AF13" password="C724"/>
+    <protectedRange name="pd93a815875f735d0c2677c827b48f71b" sqref="A14:AF14" password="C724"/>
+    <protectedRange name="pe895ab572eca41d9ec33ae95fd7a57a2" sqref="A15:AF15" password="C724"/>
+    <protectedRange name="p6e95104cf59386b416c7f67882729269" sqref="A16:AF16" password="C724"/>
+    <protectedRange name="p194dbe0bc0cbf4552237a18d857aa926" sqref="A17:AF17" password="C724"/>
+    <protectedRange name="p7b4502e0d554fce258381871a2d893a7" sqref="A18:AF18" password="C724"/>
+    <protectedRange name="p2bf8a22d7d4d479a56975070a05b7629" sqref="A19:AF19" password="C724"/>
+    <protectedRange name="p5f9d334b2e2b7d249d7fac58b63f8631" sqref="A20:AF20" password="C724"/>
+    <protectedRange name="pb3afbace8f6f7f6354d93ecb3a9b663f" sqref="A21:AF21" password="C724"/>
+    <protectedRange name="p541e80c77299ba74bfe0a8ca3ee9141d" sqref="A22:AF22" password="C724"/>
+    <protectedRange name="p23fee5e85d52e11b1d93f70d48585c2b" sqref="A23:AF23" password="C724"/>
+    <protectedRange name="pa1cabf18dd71e2ef9a7afeb8defea173" sqref="A24:AF24" password="C724"/>
+    <protectedRange name="pacef40bbf4cbf9500433f5db8b00f343" sqref="A27:AC27" password="C724"/>
+    <protectedRange name="pb2fbe0634f6ba582462d5b451e1c6da7" sqref="A29:AC29" password="C724"/>
   </protectedRanges>
   <mergeCells>
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="B12:C12"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="D12:E12"/>
     <mergeCell ref="F11:G11"/>
     <mergeCell ref="F12:G12"/>
     <mergeCell ref="H11:I11"/>
@@ -1058,9 +2039,112 @@
     <mergeCell ref="X12:AA12"/>
     <mergeCell ref="AB11:AE11"/>
     <mergeCell ref="AB12:AE12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="J13:M13"/>
+    <mergeCell ref="N13:P13"/>
+    <mergeCell ref="T13:W13"/>
+    <mergeCell ref="X13:AA13"/>
+    <mergeCell ref="AB13:AE13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="J14:M14"/>
+    <mergeCell ref="N14:P14"/>
+    <mergeCell ref="T14:W14"/>
+    <mergeCell ref="X14:AA14"/>
+    <mergeCell ref="AB14:AE14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="J15:M15"/>
+    <mergeCell ref="N15:P15"/>
+    <mergeCell ref="T15:W15"/>
+    <mergeCell ref="X15:AA15"/>
+    <mergeCell ref="AB15:AE15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="J16:M16"/>
+    <mergeCell ref="N16:P16"/>
+    <mergeCell ref="T16:W16"/>
+    <mergeCell ref="X16:AA16"/>
+    <mergeCell ref="AB16:AE16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="J17:M17"/>
+    <mergeCell ref="N17:P17"/>
+    <mergeCell ref="T17:W17"/>
+    <mergeCell ref="X17:AA17"/>
+    <mergeCell ref="AB17:AE17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="J18:M18"/>
+    <mergeCell ref="N18:P18"/>
+    <mergeCell ref="T18:W18"/>
+    <mergeCell ref="X18:AA18"/>
+    <mergeCell ref="AB18:AE18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="J19:M19"/>
+    <mergeCell ref="N19:P19"/>
+    <mergeCell ref="T19:W19"/>
+    <mergeCell ref="X19:AA19"/>
+    <mergeCell ref="AB19:AE19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="J20:M20"/>
+    <mergeCell ref="N20:P20"/>
+    <mergeCell ref="T20:W20"/>
+    <mergeCell ref="X20:AA20"/>
+    <mergeCell ref="AB20:AE20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="J21:M21"/>
+    <mergeCell ref="N21:P21"/>
+    <mergeCell ref="T21:W21"/>
+    <mergeCell ref="X21:AA21"/>
+    <mergeCell ref="AB21:AE21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="J22:M22"/>
+    <mergeCell ref="N22:P22"/>
+    <mergeCell ref="T22:W22"/>
+    <mergeCell ref="X22:AA22"/>
+    <mergeCell ref="AB22:AE22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="J23:M23"/>
+    <mergeCell ref="N23:P23"/>
+    <mergeCell ref="T23:W23"/>
+    <mergeCell ref="X23:AA23"/>
+    <mergeCell ref="AB23:AE23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="J24:M24"/>
+    <mergeCell ref="N24:P24"/>
+    <mergeCell ref="T24:W24"/>
+    <mergeCell ref="X24:AA24"/>
+    <mergeCell ref="AB24:AE24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="J25:M25"/>
+    <mergeCell ref="N25:P25"/>
+    <mergeCell ref="T25:W25"/>
+    <mergeCell ref="X25:AA25"/>
+    <mergeCell ref="AB25:AE25"/>
     <mergeCell ref="O2:T2"/>
     <mergeCell ref="B10:C10"/>
-    <mergeCell ref="D10:E10"/>
     <mergeCell ref="F10:G10"/>
     <mergeCell ref="H10:I10"/>
     <mergeCell ref="J10:M10"/>

</xml_diff>

<commit_message>
Add dr_no=''; if empty
</commit_message>
<xml_diff>
--- a/Issued Report.xlsx
+++ b/Issued Report.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="190">
   <si>
     <t>PROGEN Dieseltech Services Corp.</t>
   </si>
@@ -38,13 +38,13 @@
     <t>TO</t>
   </si>
   <si>
-    <t>2020-04-01</t>
+    <t>2020-08-01</t>
   </si>
   <si>
     <t>FROM</t>
   </si>
   <si>
-    <t>2020-06-24</t>
+    <t>2020-08-31</t>
   </si>
   <si>
     <t xml:space="preserve">Total Cost w/ PR: </t>
@@ -116,163 +116,313 @@
     <t>Frequency</t>
   </si>
   <si>
-    <t>2020-06-11</t>
-  </si>
-  <si>
-    <t>asdasd</t>
-  </si>
-  <si>
-    <t>MIF-2020-06-0006</t>
+    <t>2020-08-28</t>
+  </si>
+  <si>
+    <t>MIF-2020-08-0038</t>
+  </si>
+  <si>
+    <t>Warehouse Stocks</t>
+  </si>
+  <si>
+    <t>CON-CON_1017</t>
+  </si>
+  <si>
+    <t>Plywood, Ordinary, 4ft x 8ft x 5mm</t>
+  </si>
+  <si>
+    <t>sht/s</t>
+  </si>
+  <si>
+    <t>Progen Warehouse</t>
+  </si>
+  <si>
+    <t>Progen Consumables</t>
+  </si>
+  <si>
+    <t>Crates</t>
+  </si>
+  <si>
+    <t>CON-CON_1013</t>
+  </si>
+  <si>
+    <t>Lumber; Good, 2" x 3" x 10 ft, Mahogany</t>
+  </si>
+  <si>
+    <t>lgth/s</t>
+  </si>
+  <si>
+    <t>CON-CON_1015</t>
+  </si>
+  <si>
+    <t>Lumber: Good, 2" x 3" x 6 ft, Mahogany</t>
+  </si>
+  <si>
+    <t>2020-08-25</t>
+  </si>
+  <si>
+    <t>MIF-2020-08-0032</t>
+  </si>
+  <si>
+    <t>CON-CON_1026</t>
+  </si>
+  <si>
+    <t>Sand Paper, G1000</t>
+  </si>
+  <si>
+    <t>pc/s</t>
+  </si>
+  <si>
+    <t>ECMG</t>
+  </si>
+  <si>
+    <t>Consumables for Refurbishing  / Reconditioning</t>
+  </si>
+  <si>
+    <t>12 Units Connecting Rod Assembly and 12 Units Piston Assembly</t>
+  </si>
+  <si>
+    <t>MIF-2020-08-0033</t>
+  </si>
+  <si>
+    <t>CON-CON_1003</t>
+  </si>
+  <si>
+    <t>Sand Paper, G120</t>
+  </si>
+  <si>
+    <t>MIF-2020-08-0034</t>
+  </si>
+  <si>
+    <t>CON-HOU_1001</t>
+  </si>
+  <si>
+    <t>Rags, Cotton</t>
+  </si>
+  <si>
+    <t>kg/s</t>
+  </si>
+  <si>
+    <t>MIF-2020-08-0035</t>
+  </si>
+  <si>
+    <t>CON-FUE_1002</t>
+  </si>
+  <si>
+    <t>Penetrating Oil Multi Use, WD40</t>
+  </si>
+  <si>
+    <t>can/s</t>
+  </si>
+  <si>
+    <t>MIF-2020-08-0036</t>
+  </si>
+  <si>
+    <t>Dismantling, cleaning, inspection, crack testing, measurement &amp; evaluation, reassembling &amp; preservation.</t>
+  </si>
+  <si>
+    <t>Lateral Bolt</t>
+  </si>
+  <si>
+    <t>CON-CHE_1006</t>
+  </si>
+  <si>
+    <t>Crack Detector, Cleaner, Spotcheck, SKC-S Aerosol</t>
+  </si>
+  <si>
+    <t>CON-CHE_1007</t>
+  </si>
+  <si>
+    <t>Crack Detector, Developer, Spotcheck, SKD-S2</t>
+  </si>
+  <si>
+    <t>CON-CHE_1008</t>
+  </si>
+  <si>
+    <t>Crack Detector, Penetrant, Spotcheck, SKL-SP2</t>
+  </si>
+  <si>
+    <t>MIF-2020-08-0037</t>
+  </si>
+  <si>
+    <t>Intermediate Gear, Crankshaft Gear, Bearing Body and Lateral Bolt</t>
+  </si>
+  <si>
+    <t>2020-08-24</t>
+  </si>
+  <si>
+    <t>MIF-2020-08-0031</t>
+  </si>
+  <si>
+    <t>WHP20-1027 / PROGEN-010-2020</t>
+  </si>
+  <si>
+    <t>CON-HOU_1003</t>
+  </si>
+  <si>
+    <t>Gloves, Cotton</t>
+  </si>
+  <si>
+    <t>pair/s</t>
+  </si>
+  <si>
+    <t>Personal Protective Equipment</t>
+  </si>
+  <si>
+    <t>36 Units SEMT Pielstick PC2-5 Cylinder Head Assembly</t>
+  </si>
+  <si>
+    <t>2020-08-22</t>
+  </si>
+  <si>
+    <t>MIF-2020-08-0029</t>
+  </si>
+  <si>
+    <t>WHP20-1035 / PROGEN-018-2020</t>
+  </si>
+  <si>
+    <t>CON-FUE_1001</t>
+  </si>
+  <si>
+    <t>Diesel, Fuel-Save</t>
+  </si>
+  <si>
+    <t>ltr/s</t>
+  </si>
+  <si>
+    <t>MIF-2020-08-0030</t>
+  </si>
+  <si>
+    <t>2020-08-19</t>
+  </si>
+  <si>
+    <t>MIF-2020-08-0028</t>
+  </si>
+  <si>
+    <t>WHP20-1038 / PROGEN-023-2020</t>
+  </si>
+  <si>
+    <t>CON-CON_1039</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Instant Adhesive, 495, 20g </t>
+  </si>
+  <si>
+    <t>2020-08-18</t>
+  </si>
+  <si>
+    <t>MIF-2020-08-0026</t>
   </si>
   <si>
     <t>PRO20-1002</t>
   </si>
   <si>
-    <t>PRO-PF 128-30C</t>
-  </si>
-  <si>
-    <t>"Express" Union</t>
-  </si>
-  <si>
-    <t>pc/s</t>
-  </si>
-  <si>
-    <t>Progen Warehouse</t>
-  </si>
-  <si>
-    <t>Progen Consumables</t>
+    <t>CON-OFF_1009</t>
+  </si>
+  <si>
+    <t>Scotch Tape, Clear, 2"</t>
+  </si>
+  <si>
+    <t>roll/s</t>
   </si>
   <si>
     <t>Progen Personnel &amp; Helper</t>
   </si>
   <si>
-    <t>2020-06-10</t>
-  </si>
-  <si>
-    <t>MIF-2020-06-0001</t>
-  </si>
-  <si>
-    <t>CON-HOU_1001</t>
-  </si>
-  <si>
-    <t>Rags, Cotton</t>
-  </si>
-  <si>
-    <t>kg/s</t>
-  </si>
-  <si>
-    <t>2020-05-18</t>
-  </si>
-  <si>
-    <t>MIF-2020-05-0007</t>
-  </si>
-  <si>
-    <t>CON-OFF_1006</t>
-  </si>
-  <si>
-    <t>Pencil, Mongol #2</t>
-  </si>
-  <si>
-    <t>2020-05-16</t>
-  </si>
-  <si>
-    <t>MIF-2020-05-0006</t>
-  </si>
-  <si>
-    <t>EIC20-1006</t>
-  </si>
-  <si>
-    <t>EIC-PAR_1001</t>
-  </si>
-  <si>
-    <t>Potential Transformer, Part Number: PTW4-2-75-722FF, Part ID: 109562</t>
-  </si>
-  <si>
-    <t>unit/s</t>
-  </si>
-  <si>
-    <t>EIC</t>
-  </si>
-  <si>
-    <t>Replacement of Defective Generator Potential Transformer</t>
-  </si>
-  <si>
-    <t>DG2 Running Unit</t>
-  </si>
-  <si>
-    <t>2020-05-14</t>
-  </si>
-  <si>
-    <t>MIF-2020-05-0005</t>
-  </si>
-  <si>
-    <t>CON-OFF_1010</t>
-  </si>
-  <si>
-    <t>Bondpaper, A4</t>
-  </si>
-  <si>
-    <t>ream/s</t>
-  </si>
-  <si>
-    <t>CON-OFF_1007</t>
-  </si>
-  <si>
-    <t>Ink Refill for Permanent Marker, Black</t>
-  </si>
-  <si>
-    <t>2020-05-12</t>
-  </si>
-  <si>
-    <t>MIF-2020-05-0004</t>
-  </si>
-  <si>
-    <t>WHP20-1001</t>
-  </si>
-  <si>
-    <t>Progen CV</t>
-  </si>
-  <si>
-    <t>Dismantling, cleaning, inspection, crack testing, measurement &amp; evaluation, reassembling &amp; preservation.</t>
-  </si>
-  <si>
-    <t>DG4 (CV Area) Main Engine Parts &amp; Components</t>
-  </si>
-  <si>
-    <t>2020-05-05</t>
-  </si>
-  <si>
-    <t>MIF-2020-05-0001</t>
-  </si>
-  <si>
-    <t>CON-OFF_1013</t>
-  </si>
-  <si>
-    <t>Cutter Blade Refill ( 1 box=10 pcs)</t>
-  </si>
-  <si>
-    <t>box/s</t>
-  </si>
-  <si>
-    <t>MIF-2020-05-0002</t>
-  </si>
-  <si>
-    <t>CON-OFF_1012</t>
-  </si>
-  <si>
-    <t>Paper Clip, 33mm</t>
-  </si>
-  <si>
-    <t>MIF-2020-05-0003</t>
-  </si>
-  <si>
-    <t>PROGEN-008-2019</t>
-  </si>
-  <si>
-    <t>CON-OFF_1005</t>
-  </si>
-  <si>
-    <t>Tape, Masking 1"</t>
+    <t>MIF-2020-08-0027</t>
+  </si>
+  <si>
+    <t>CON-CHE_1001</t>
+  </si>
+  <si>
+    <t>Vappro 868 VCI Corrosion Inhibitor Wax Coating (4 liters/gallon)</t>
+  </si>
+  <si>
+    <t>gal/s</t>
+  </si>
+  <si>
+    <t>2020-08-17</t>
+  </si>
+  <si>
+    <t>MIF-2020-08-0024</t>
+  </si>
+  <si>
+    <t>REC20-1012 / PROGEN-009-2020</t>
+  </si>
+  <si>
+    <t>CON-OEA_1003</t>
+  </si>
+  <si>
+    <t>Grinding Compound, Silicon Carbide, Grade E, Grit 120, Coarse, 16 oz.</t>
+  </si>
+  <si>
+    <t>MIF-2020-08-0025</t>
+  </si>
+  <si>
+    <t>CON-OFF_1002</t>
+  </si>
+  <si>
+    <t>Tape, Masking 2"</t>
+  </si>
+  <si>
+    <t>2020-08-15</t>
+  </si>
+  <si>
+    <t>MIF-2020-08-0023</t>
+  </si>
+  <si>
+    <t>2020-08-14</t>
+  </si>
+  <si>
+    <t>MIF-2020-08-0021</t>
+  </si>
+  <si>
+    <t>begbal123119</t>
+  </si>
+  <si>
+    <t>MIF-2020-08-0022</t>
+  </si>
+  <si>
+    <t>Inventory Beginning Balance</t>
+  </si>
+  <si>
+    <t>Warehouse Beginning Balance</t>
+  </si>
+  <si>
+    <t>2020-08-13</t>
+  </si>
+  <si>
+    <t>MIF-2020-08-0020</t>
+  </si>
+  <si>
+    <t>REC20-1011 / PROGEN-009-2020</t>
+  </si>
+  <si>
+    <t>2020-08-11</t>
+  </si>
+  <si>
+    <t>MIF-2020-08-0019</t>
+  </si>
+  <si>
+    <t>CON-CON_1001</t>
+  </si>
+  <si>
+    <t>Scraper, Industrial; Size: 2"</t>
+  </si>
+  <si>
+    <t>2020-08-10</t>
+  </si>
+  <si>
+    <t>MIF-2020-08-0015</t>
+  </si>
+  <si>
+    <t>PROGEN-004-2019</t>
+  </si>
+  <si>
+    <t>CON-CHE_1004</t>
+  </si>
+  <si>
+    <t>Acid; Muriatic</t>
   </si>
   <si>
     <t>Consumables / Cleaning &amp; Preservation of Spare parts</t>
@@ -282,37 +432,142 @@
 </t>
   </si>
   <si>
-    <t>2020-04-28</t>
-  </si>
-  <si>
-    <t>MIF-2020-04-0040</t>
-  </si>
-  <si>
-    <t>2020-04-06</t>
-  </si>
-  <si>
-    <t>MIF-2020-04-0039</t>
-  </si>
-  <si>
-    <t>CON-OFF_1003</t>
-  </si>
-  <si>
-    <t>Tape, Cellophane, 1"</t>
-  </si>
-  <si>
-    <t>2020-04-04</t>
-  </si>
-  <si>
-    <t>MIF-2020-04-0038</t>
-  </si>
-  <si>
-    <t>PROR-133-2019</t>
-  </si>
-  <si>
-    <t>CON-OFF_1002</t>
-  </si>
-  <si>
-    <t>Tape, Masking 2"</t>
+    <t>MIF-2020-08-0016</t>
+  </si>
+  <si>
+    <t>WHP20-1000</t>
+  </si>
+  <si>
+    <t>CON-OFF_1016</t>
+  </si>
+  <si>
+    <t>Tape, Duct: Multi-Use, #2945, 1.88Inx45YD(48mmx41.1m)</t>
+  </si>
+  <si>
+    <t>MIF-2020-08-0017</t>
+  </si>
+  <si>
+    <t>PRO20-1004</t>
+  </si>
+  <si>
+    <t>CON-OFF_1005</t>
+  </si>
+  <si>
+    <t>Tape, Masking 1"</t>
+  </si>
+  <si>
+    <t>Office Supplies</t>
+  </si>
+  <si>
+    <t>Progen Office Use</t>
+  </si>
+  <si>
+    <t>MIF-2020-08-0018</t>
+  </si>
+  <si>
+    <t>2020-08-08</t>
+  </si>
+  <si>
+    <t>MIF-2020-08-0013</t>
+  </si>
+  <si>
+    <t>MIF-2020-08-0014</t>
+  </si>
+  <si>
+    <t>WHP20-1037 / PROGEN-021-2020</t>
+  </si>
+  <si>
+    <t>CON-OFF_1001</t>
+  </si>
+  <si>
+    <t>Marker, Metal, Color: Yellow</t>
+  </si>
+  <si>
+    <t>2020-08-07</t>
+  </si>
+  <si>
+    <t>MIF-2020-08-0012</t>
+  </si>
+  <si>
+    <t>2020-08-06</t>
+  </si>
+  <si>
+    <t>MIF-2020-08-0011</t>
+  </si>
+  <si>
+    <t>CON-CON_1018</t>
+  </si>
+  <si>
+    <t>Tie Wire, #16</t>
+  </si>
+  <si>
+    <t>Equipment @ CV yard</t>
+  </si>
+  <si>
+    <t>2020-08-05</t>
+  </si>
+  <si>
+    <t>MIF-2020-08-0005</t>
+  </si>
+  <si>
+    <t>MIF-2020-08-0006</t>
+  </si>
+  <si>
+    <t>WHP20-1026</t>
+  </si>
+  <si>
+    <t>CON-HOU_1006</t>
+  </si>
+  <si>
+    <t>Soap, liquid</t>
+  </si>
+  <si>
+    <t>MIF-2020-08-0007</t>
+  </si>
+  <si>
+    <t>MIF-2020-08-0008</t>
+  </si>
+  <si>
+    <t>WHP20-1033 / PROGEN-016-2020</t>
+  </si>
+  <si>
+    <t>CON-CON_1037</t>
+  </si>
+  <si>
+    <t>Bag; Garbage, Size: XXL, (1 roll = 10 pcs.)</t>
+  </si>
+  <si>
+    <t>MIF-2020-08-0009</t>
+  </si>
+  <si>
+    <t>CON-CON_1021</t>
+  </si>
+  <si>
+    <t>Metal Polish, A1</t>
+  </si>
+  <si>
+    <t>MIF-2020-08-0010</t>
+  </si>
+  <si>
+    <t>2020-08-04</t>
+  </si>
+  <si>
+    <t>MIF-2020-08-0001</t>
+  </si>
+  <si>
+    <t>CON-OFF_1017</t>
+  </si>
+  <si>
+    <t>Pen, Ballpoint, Black</t>
+  </si>
+  <si>
+    <t>MIF-2020-08-0002</t>
+  </si>
+  <si>
+    <t>MIF-2020-08-0003</t>
+  </si>
+  <si>
+    <t>MIF-2020-08-0004</t>
   </si>
   <si>
     <t xml:space="preserve">Prepared By: </t>
@@ -839,7 +1094,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:AF29"/>
+  <dimension ref="A1:AF65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="O2" sqref="O2"/>
@@ -1016,7 +1271,7 @@
       </c>
       <c r="R5" s="1"/>
       <c r="S5" s="1">
-        <v>789.3</v>
+        <v>26844.2</v>
       </c>
       <c r="T5" s="1"/>
       <c r="U5" s="1"/>
@@ -1024,7 +1279,7 @@
         <v>11</v>
       </c>
       <c r="Z5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:32">
@@ -1033,7 +1288,7 @@
       </c>
       <c r="R6" s="1"/>
       <c r="S6" s="1">
-        <v>0</v>
+        <v>19993.5</v>
       </c>
       <c r="T6" s="1"/>
       <c r="U6" s="1"/>
@@ -1041,7 +1296,7 @@
         <v>13</v>
       </c>
       <c r="Z6">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:32">
@@ -1141,54 +1396,52 @@
         <v>33</v>
       </c>
       <c r="C11" s="4"/>
-      <c r="D11" s="2" t="s">
+      <c r="D11" s="2"/>
+      <c r="E11" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="F11" s="2" t="s">
         <v>35</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>36</v>
       </c>
       <c r="G11" s="2"/>
       <c r="H11" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I11" s="2"/>
       <c r="J11" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K11" s="2"/>
       <c r="L11" s="2"/>
       <c r="M11" s="2"/>
       <c r="N11" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O11" s="5"/>
       <c r="P11" s="5"/>
       <c r="Q11" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="R11" s="5">
+        <v>450</v>
+      </c>
+      <c r="S11" s="4">
+        <v>900</v>
+      </c>
+      <c r="T11" s="2" t="s">
         <v>39</v>
-      </c>
-      <c r="R11" s="5">
-        <v>200</v>
-      </c>
-      <c r="S11" s="4">
-        <v>200</v>
-      </c>
-      <c r="T11" s="2" t="s">
-        <v>40</v>
       </c>
       <c r="U11" s="2"/>
       <c r="V11" s="2"/>
       <c r="W11" s="2"/>
       <c r="X11" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Y11" s="2"/>
       <c r="Z11" s="2"/>
       <c r="AA11" s="2"/>
       <c r="AB11" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AC11" s="2"/>
       <c r="AD11" s="2"/>
@@ -1200,57 +1453,55 @@
         <v>2</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="C12" s="4"/>
-      <c r="D12" s="2">
-        <v>1022</v>
-      </c>
+      <c r="D12" s="2"/>
       <c r="E12" s="2" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G12" s="2"/>
       <c r="H12" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="I12" s="2"/>
       <c r="J12" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
       <c r="M12" s="2"/>
       <c r="N12" s="5">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="O12" s="5"/>
       <c r="P12" s="5"/>
       <c r="Q12" s="5" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="R12" s="5">
-        <v>50</v>
+        <v>275</v>
       </c>
       <c r="S12" s="4">
-        <v>50</v>
+        <v>1375</v>
       </c>
       <c r="T12" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="U12" s="2"/>
       <c r="V12" s="2"/>
       <c r="W12" s="2"/>
       <c r="X12" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Y12" s="2"/>
       <c r="Z12" s="2"/>
       <c r="AA12" s="2"/>
       <c r="AB12" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AC12" s="2"/>
       <c r="AD12" s="2"/>
@@ -1262,57 +1513,55 @@
         <v>3</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="C13" s="4"/>
-      <c r="D13" s="2">
-        <v>1000</v>
-      </c>
+      <c r="D13" s="2"/>
       <c r="E13" s="2" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G13" s="2"/>
       <c r="H13" s="2" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="I13" s="2"/>
       <c r="J13" s="2" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="K13" s="2"/>
       <c r="L13" s="2"/>
       <c r="M13" s="2"/>
       <c r="N13" s="5">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="O13" s="5"/>
       <c r="P13" s="5"/>
       <c r="Q13" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="R13" s="5">
+        <v>150</v>
+      </c>
+      <c r="S13" s="4">
+        <v>900</v>
+      </c>
+      <c r="T13" s="2" t="s">
         <v>39</v>
-      </c>
-      <c r="R13" s="5">
-        <v>5.8</v>
-      </c>
-      <c r="S13" s="4">
-        <v>5.8</v>
-      </c>
-      <c r="T13" s="2" t="s">
-        <v>40</v>
       </c>
       <c r="U13" s="2"/>
       <c r="V13" s="2"/>
       <c r="W13" s="2"/>
       <c r="X13" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Y13" s="2"/>
       <c r="Z13" s="2"/>
       <c r="AA13" s="2"/>
       <c r="AB13" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AC13" s="2"/>
       <c r="AD13" s="2"/>
@@ -1324,57 +1573,55 @@
         <v>4</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C14" s="4"/>
-      <c r="D14" s="2">
-        <v>1011</v>
-      </c>
+      <c r="D14" s="2"/>
       <c r="E14" s="2" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>54</v>
+        <v>35</v>
       </c>
       <c r="G14" s="2"/>
       <c r="H14" s="2" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="I14" s="2"/>
       <c r="J14" s="2" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
       <c r="M14" s="2"/>
       <c r="N14" s="5">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="O14" s="5"/>
       <c r="P14" s="5"/>
       <c r="Q14" s="5" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="R14" s="5">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="S14" s="4">
-        <v>0</v>
+        <v>110</v>
       </c>
       <c r="T14" s="2" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="U14" s="2"/>
       <c r="V14" s="2"/>
       <c r="W14" s="2"/>
       <c r="X14" s="2" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="Y14" s="2"/>
       <c r="Z14" s="2"/>
       <c r="AA14" s="2"/>
       <c r="AB14" s="2" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="AC14" s="2"/>
       <c r="AD14" s="2"/>
@@ -1386,57 +1633,55 @@
         <v>5</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
       <c r="C15" s="4"/>
-      <c r="D15" s="2">
-        <v>1001</v>
-      </c>
+      <c r="D15" s="2"/>
       <c r="E15" s="2" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G15" s="2"/>
       <c r="H15" s="2" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="I15" s="2"/>
       <c r="J15" s="2" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="K15" s="2"/>
       <c r="L15" s="2"/>
       <c r="M15" s="2"/>
       <c r="N15" s="5">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="O15" s="5"/>
       <c r="P15" s="5"/>
       <c r="Q15" s="5" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="R15" s="5">
-        <v>170</v>
+        <v>14</v>
       </c>
       <c r="S15" s="4">
-        <v>170</v>
+        <v>280</v>
       </c>
       <c r="T15" s="2" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="U15" s="2"/>
       <c r="V15" s="2"/>
       <c r="W15" s="2"/>
       <c r="X15" s="2" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="Y15" s="2"/>
       <c r="Z15" s="2"/>
       <c r="AA15" s="2"/>
       <c r="AB15" s="2" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="AC15" s="2"/>
       <c r="AD15" s="2"/>
@@ -1448,25 +1693,23 @@
         <v>6</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
       <c r="C16" s="4"/>
-      <c r="D16" s="2">
-        <v>1000</v>
-      </c>
+      <c r="D16" s="2"/>
       <c r="E16" s="2" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G16" s="2"/>
       <c r="H16" s="2" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="I16" s="2"/>
       <c r="J16" s="2" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="K16" s="2"/>
       <c r="L16" s="2"/>
@@ -1477,28 +1720,28 @@
       <c r="O16" s="5"/>
       <c r="P16" s="5"/>
       <c r="Q16" s="5" t="s">
-        <v>39</v>
+        <v>61</v>
       </c>
       <c r="R16" s="5">
-        <v>72</v>
+        <v>50</v>
       </c>
       <c r="S16" s="4">
-        <v>72</v>
+        <v>50</v>
       </c>
       <c r="T16" s="2" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="U16" s="2"/>
       <c r="V16" s="2"/>
       <c r="W16" s="2"/>
       <c r="X16" s="2" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="Y16" s="2"/>
       <c r="Z16" s="2"/>
       <c r="AA16" s="2"/>
       <c r="AB16" s="2" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="AC16" s="2"/>
       <c r="AD16" s="2"/>
@@ -1510,57 +1753,55 @@
         <v>7</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>68</v>
+        <v>47</v>
       </c>
       <c r="C17" s="4"/>
-      <c r="D17" s="2">
-        <v>1009</v>
-      </c>
+      <c r="D17" s="2"/>
       <c r="E17" s="2" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>70</v>
+        <v>35</v>
       </c>
       <c r="G17" s="2"/>
       <c r="H17" s="2" t="s">
-        <v>45</v>
+        <v>63</v>
       </c>
       <c r="I17" s="2"/>
       <c r="J17" s="2" t="s">
-        <v>46</v>
+        <v>64</v>
       </c>
       <c r="K17" s="2"/>
       <c r="L17" s="2"/>
       <c r="M17" s="2"/>
       <c r="N17" s="5">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="O17" s="5"/>
       <c r="P17" s="5"/>
       <c r="Q17" s="5" t="s">
-        <v>47</v>
+        <v>65</v>
       </c>
       <c r="R17" s="5">
-        <v>50</v>
+        <v>210</v>
       </c>
       <c r="S17" s="4">
-        <v>100</v>
+        <v>1050</v>
       </c>
       <c r="T17" s="2" t="s">
-        <v>71</v>
+        <v>52</v>
       </c>
       <c r="U17" s="2"/>
       <c r="V17" s="2"/>
       <c r="W17" s="2"/>
       <c r="X17" s="2" t="s">
-        <v>72</v>
+        <v>53</v>
       </c>
       <c r="Y17" s="2"/>
       <c r="Z17" s="2"/>
       <c r="AA17" s="2"/>
       <c r="AB17" s="2" t="s">
-        <v>73</v>
+        <v>54</v>
       </c>
       <c r="AC17" s="2"/>
       <c r="AD17" s="2"/>
@@ -1572,57 +1813,53 @@
         <v>8</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>74</v>
+        <v>47</v>
       </c>
       <c r="C18" s="4"/>
-      <c r="D18" s="2">
-        <v>1005</v>
-      </c>
+      <c r="D18" s="2"/>
       <c r="E18" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>36</v>
-      </c>
+        <v>66</v>
+      </c>
+      <c r="F18" s="2"/>
       <c r="G18" s="2"/>
       <c r="H18" s="2" t="s">
-        <v>76</v>
+        <v>59</v>
       </c>
       <c r="I18" s="2"/>
       <c r="J18" s="2" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
       <c r="K18" s="2"/>
       <c r="L18" s="2"/>
       <c r="M18" s="2"/>
       <c r="N18" s="5">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="O18" s="5"/>
       <c r="P18" s="5"/>
       <c r="Q18" s="5" t="s">
-        <v>78</v>
+        <v>61</v>
       </c>
       <c r="R18" s="5">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="S18" s="4">
         <v>25</v>
       </c>
       <c r="T18" s="2" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="U18" s="2"/>
       <c r="V18" s="2"/>
       <c r="W18" s="2"/>
       <c r="X18" s="2" t="s">
-        <v>41</v>
+        <v>67</v>
       </c>
       <c r="Y18" s="2"/>
       <c r="Z18" s="2"/>
       <c r="AA18" s="2"/>
       <c r="AB18" s="2" t="s">
-        <v>42</v>
+        <v>68</v>
       </c>
       <c r="AC18" s="2"/>
       <c r="AD18" s="2"/>
@@ -1634,25 +1871,21 @@
         <v>9</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>74</v>
+        <v>47</v>
       </c>
       <c r="C19" s="4"/>
-      <c r="D19" s="2">
-        <v>1001</v>
-      </c>
+      <c r="D19" s="2"/>
       <c r="E19" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>36</v>
-      </c>
+        <v>66</v>
+      </c>
+      <c r="F19" s="2"/>
       <c r="G19" s="2"/>
       <c r="H19" s="2" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="I19" s="2"/>
       <c r="J19" s="2" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="K19" s="2"/>
       <c r="L19" s="2"/>
@@ -1663,28 +1896,28 @@
       <c r="O19" s="5"/>
       <c r="P19" s="5"/>
       <c r="Q19" s="5" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
       <c r="R19" s="5">
-        <v>7.5</v>
+        <v>610</v>
       </c>
       <c r="S19" s="4">
-        <v>7.5</v>
+        <v>610</v>
       </c>
       <c r="T19" s="2" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="U19" s="2"/>
       <c r="V19" s="2"/>
       <c r="W19" s="2"/>
       <c r="X19" s="2" t="s">
-        <v>41</v>
+        <v>67</v>
       </c>
       <c r="Y19" s="2"/>
       <c r="Z19" s="2"/>
       <c r="AA19" s="2"/>
       <c r="AB19" s="2" t="s">
-        <v>42</v>
+        <v>68</v>
       </c>
       <c r="AC19" s="2"/>
       <c r="AD19" s="2"/>
@@ -1696,25 +1929,21 @@
         <v>10</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>74</v>
+        <v>47</v>
       </c>
       <c r="C20" s="4"/>
-      <c r="D20" s="2">
-        <v>72</v>
-      </c>
+      <c r="D20" s="2"/>
       <c r="E20" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>83</v>
-      </c>
+        <v>66</v>
+      </c>
+      <c r="F20" s="2"/>
       <c r="G20" s="2"/>
       <c r="H20" s="2" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="I20" s="2"/>
       <c r="J20" s="2" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="K20" s="2"/>
       <c r="L20" s="2"/>
@@ -1725,28 +1954,28 @@
       <c r="O20" s="5"/>
       <c r="P20" s="5"/>
       <c r="Q20" s="5" t="s">
-        <v>39</v>
+        <v>65</v>
       </c>
       <c r="R20" s="5">
-        <v>31</v>
+        <v>750</v>
       </c>
       <c r="S20" s="4">
-        <v>31</v>
+        <v>750</v>
       </c>
       <c r="T20" s="2" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="U20" s="2"/>
       <c r="V20" s="2"/>
       <c r="W20" s="2"/>
       <c r="X20" s="2" t="s">
-        <v>86</v>
+        <v>67</v>
       </c>
       <c r="Y20" s="2"/>
       <c r="Z20" s="2"/>
       <c r="AA20" s="2"/>
       <c r="AB20" s="2" t="s">
-        <v>87</v>
+        <v>68</v>
       </c>
       <c r="AC20" s="2"/>
       <c r="AD20" s="2"/>
@@ -1758,25 +1987,21 @@
         <v>11</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>88</v>
+        <v>47</v>
       </c>
       <c r="C21" s="4"/>
-      <c r="D21" s="2">
-        <v>1009</v>
-      </c>
+      <c r="D21" s="2"/>
       <c r="E21" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>70</v>
-      </c>
+        <v>66</v>
+      </c>
+      <c r="F21" s="2"/>
       <c r="G21" s="2"/>
       <c r="H21" s="2" t="s">
-        <v>45</v>
+        <v>73</v>
       </c>
       <c r="I21" s="2"/>
       <c r="J21" s="2" t="s">
-        <v>46</v>
+        <v>74</v>
       </c>
       <c r="K21" s="2"/>
       <c r="L21" s="2"/>
@@ -1787,28 +2012,28 @@
       <c r="O21" s="5"/>
       <c r="P21" s="5"/>
       <c r="Q21" s="5" t="s">
-        <v>47</v>
+        <v>65</v>
       </c>
       <c r="R21" s="5">
-        <v>50</v>
+        <v>750</v>
       </c>
       <c r="S21" s="4">
-        <v>50</v>
+        <v>750</v>
       </c>
       <c r="T21" s="2" t="s">
-        <v>71</v>
+        <v>52</v>
       </c>
       <c r="U21" s="2"/>
       <c r="V21" s="2"/>
       <c r="W21" s="2"/>
       <c r="X21" s="2" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="Y21" s="2"/>
       <c r="Z21" s="2"/>
       <c r="AA21" s="2"/>
       <c r="AB21" s="2" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="AC21" s="2"/>
       <c r="AD21" s="2"/>
@@ -1820,57 +2045,53 @@
         <v>12</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>90</v>
+        <v>47</v>
       </c>
       <c r="C22" s="4"/>
-      <c r="D22" s="2">
-        <v>72</v>
-      </c>
+      <c r="D22" s="2"/>
       <c r="E22" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>83</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="F22" s="2"/>
       <c r="G22" s="2"/>
       <c r="H22" s="2" t="s">
-        <v>92</v>
+        <v>69</v>
       </c>
       <c r="I22" s="2"/>
       <c r="J22" s="2" t="s">
-        <v>93</v>
+        <v>70</v>
       </c>
       <c r="K22" s="2"/>
       <c r="L22" s="2"/>
       <c r="M22" s="2"/>
       <c r="N22" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O22" s="5"/>
       <c r="P22" s="5"/>
       <c r="Q22" s="5" t="s">
-        <v>39</v>
+        <v>65</v>
       </c>
       <c r="R22" s="5">
-        <v>17</v>
+        <v>610</v>
       </c>
       <c r="S22" s="4">
-        <v>17</v>
+        <v>1220</v>
       </c>
       <c r="T22" s="2" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="U22" s="2"/>
       <c r="V22" s="2"/>
       <c r="W22" s="2"/>
       <c r="X22" s="2" t="s">
-        <v>86</v>
+        <v>67</v>
       </c>
       <c r="Y22" s="2"/>
       <c r="Z22" s="2"/>
       <c r="AA22" s="2"/>
       <c r="AB22" s="2" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="AC22" s="2"/>
       <c r="AD22" s="2"/>
@@ -1882,57 +2103,53 @@
         <v>13</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>94</v>
+        <v>47</v>
       </c>
       <c r="C23" s="4"/>
-      <c r="D23" s="2">
-        <v>5</v>
-      </c>
+      <c r="D23" s="2"/>
       <c r="E23" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>96</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="F23" s="2"/>
       <c r="G23" s="2"/>
       <c r="H23" s="2" t="s">
-        <v>97</v>
+        <v>71</v>
       </c>
       <c r="I23" s="2"/>
       <c r="J23" s="2" t="s">
-        <v>98</v>
+        <v>72</v>
       </c>
       <c r="K23" s="2"/>
       <c r="L23" s="2"/>
       <c r="M23" s="2"/>
       <c r="N23" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O23" s="5"/>
       <c r="P23" s="5"/>
       <c r="Q23" s="5" t="s">
-        <v>39</v>
+        <v>65</v>
       </c>
       <c r="R23" s="5">
-        <v>61</v>
+        <v>750</v>
       </c>
       <c r="S23" s="4">
-        <v>61</v>
+        <v>1500</v>
       </c>
       <c r="T23" s="2" t="s">
-        <v>71</v>
+        <v>52</v>
       </c>
       <c r="U23" s="2"/>
       <c r="V23" s="2"/>
       <c r="W23" s="2"/>
       <c r="X23" s="2" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="Y23" s="2"/>
       <c r="Z23" s="2"/>
       <c r="AA23" s="2"/>
       <c r="AB23" s="2" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="AC23" s="2"/>
       <c r="AD23" s="2"/>
@@ -1940,55 +2157,2265 @@
       <c r="AF23" s="2"/>
     </row>
     <row r="24" spans="1:32">
-      <c r="B24" s="3"/>
-      <c r="C24" s="3"/>
-      <c r="F24"/>
-      <c r="G24"/>
-      <c r="H24"/>
-      <c r="I24"/>
-      <c r="J24"/>
-      <c r="K24"/>
-      <c r="L24"/>
-      <c r="M24"/>
-      <c r="N24" s="3"/>
-      <c r="O24" s="3"/>
-      <c r="P24" s="3"/>
-      <c r="Q24" s="3"/>
-      <c r="R24" s="3"/>
-      <c r="S24" s="3"/>
-      <c r="T24"/>
-      <c r="U24"/>
-      <c r="V24"/>
-      <c r="W24"/>
-      <c r="X24"/>
-      <c r="Y24"/>
-      <c r="Z24"/>
-      <c r="AA24"/>
-      <c r="AB24"/>
-      <c r="AC24"/>
-      <c r="AD24"/>
-      <c r="AE24"/>
+      <c r="A24" s="2">
+        <v>14</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C24" s="4"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="K24" s="2"/>
+      <c r="L24" s="2"/>
+      <c r="M24" s="2"/>
+      <c r="N24" s="5">
+        <v>2</v>
+      </c>
+      <c r="O24" s="5"/>
+      <c r="P24" s="5"/>
+      <c r="Q24" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="R24" s="5">
+        <v>750</v>
+      </c>
+      <c r="S24" s="4">
+        <v>1500</v>
+      </c>
+      <c r="T24" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="U24" s="2"/>
+      <c r="V24" s="2"/>
+      <c r="W24" s="2"/>
+      <c r="X24" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="Y24" s="2"/>
+      <c r="Z24" s="2"/>
+      <c r="AA24" s="2"/>
+      <c r="AB24" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="AC24" s="2"/>
+      <c r="AD24" s="2"/>
+      <c r="AE24" s="2"/>
+      <c r="AF24" s="2"/>
+    </row>
+    <row r="25" spans="1:32">
+      <c r="A25" s="2">
+        <v>15</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C25" s="4"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="I25" s="2"/>
+      <c r="J25" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="K25" s="2"/>
+      <c r="L25" s="2"/>
+      <c r="M25" s="2"/>
+      <c r="N25" s="5">
+        <v>2</v>
+      </c>
+      <c r="O25" s="5"/>
+      <c r="P25" s="5"/>
+      <c r="Q25" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="R25" s="5">
+        <v>50</v>
+      </c>
+      <c r="S25" s="4">
+        <v>100</v>
+      </c>
+      <c r="T25" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="U25" s="2"/>
+      <c r="V25" s="2"/>
+      <c r="W25" s="2"/>
+      <c r="X25" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="Y25" s="2"/>
+      <c r="Z25" s="2"/>
+      <c r="AA25" s="2"/>
+      <c r="AB25" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="AC25" s="2"/>
+      <c r="AD25" s="2"/>
+      <c r="AE25" s="2"/>
+      <c r="AF25" s="2"/>
     </row>
     <row r="26" spans="1:32">
-      <c r="A26" t="s">
+      <c r="A26" s="2">
+        <v>16</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C26" s="4"/>
+      <c r="D26" s="2">
+        <v>1096</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="I26" s="2"/>
+      <c r="J26" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="K26" s="2"/>
+      <c r="L26" s="2"/>
+      <c r="M26" s="2"/>
+      <c r="N26" s="5">
+        <v>28</v>
+      </c>
+      <c r="O26" s="5"/>
+      <c r="P26" s="5"/>
+      <c r="Q26" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="R26" s="5">
+        <v>11.45</v>
+      </c>
+      <c r="S26" s="4">
+        <v>320.6</v>
+      </c>
+      <c r="T26" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="U26" s="2"/>
+      <c r="V26" s="2"/>
+      <c r="W26" s="2"/>
+      <c r="X26" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="Y26" s="2"/>
+      <c r="Z26" s="2"/>
+      <c r="AA26" s="2"/>
+      <c r="AB26" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="AC26" s="2"/>
+      <c r="AD26" s="2"/>
+      <c r="AE26" s="2"/>
+      <c r="AF26" s="2"/>
+    </row>
+    <row r="27" spans="1:32">
+      <c r="A27" s="2">
+        <v>17</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C27" s="4"/>
+      <c r="D27" s="2">
+        <v>1107</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="K27" s="2"/>
+      <c r="L27" s="2"/>
+      <c r="M27" s="2"/>
+      <c r="N27" s="5">
+        <v>10</v>
+      </c>
+      <c r="O27" s="5"/>
+      <c r="P27" s="5"/>
+      <c r="Q27" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="R27" s="5">
+        <v>34.21</v>
+      </c>
+      <c r="S27" s="4">
+        <v>342.1</v>
+      </c>
+      <c r="T27" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="U27" s="2"/>
+      <c r="V27" s="2"/>
+      <c r="W27" s="2"/>
+      <c r="X27" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="Y27" s="2"/>
+      <c r="Z27" s="2"/>
+      <c r="AA27" s="2"/>
+      <c r="AB27" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="AC27" s="2"/>
+      <c r="AD27" s="2"/>
+      <c r="AE27" s="2"/>
+      <c r="AF27" s="2"/>
+    </row>
+    <row r="28" spans="1:32">
+      <c r="A28" s="2">
+        <v>18</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C28" s="4"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="I28" s="2"/>
+      <c r="J28" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="K28" s="2"/>
+      <c r="L28" s="2"/>
+      <c r="M28" s="2"/>
+      <c r="N28" s="5">
+        <v>2</v>
+      </c>
+      <c r="O28" s="5"/>
+      <c r="P28" s="5"/>
+      <c r="Q28" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="R28" s="5">
+        <v>450</v>
+      </c>
+      <c r="S28" s="4">
+        <v>900</v>
+      </c>
+      <c r="T28" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="U28" s="2"/>
+      <c r="V28" s="2"/>
+      <c r="W28" s="2"/>
+      <c r="X28" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y28" s="2"/>
+      <c r="Z28" s="2"/>
+      <c r="AA28" s="2"/>
+      <c r="AB28" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="AC28" s="2"/>
+      <c r="AD28" s="2"/>
+      <c r="AE28" s="2"/>
+      <c r="AF28" s="2"/>
+    </row>
+    <row r="29" spans="1:32">
+      <c r="A29" s="2">
+        <v>19</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C29" s="4"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G29" s="2"/>
+      <c r="H29" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="I29" s="2"/>
+      <c r="J29" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="K29" s="2"/>
+      <c r="L29" s="2"/>
+      <c r="M29" s="2"/>
+      <c r="N29" s="5">
+        <v>4</v>
+      </c>
+      <c r="O29" s="5"/>
+      <c r="P29" s="5"/>
+      <c r="Q29" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="R29" s="5">
+        <v>275</v>
+      </c>
+      <c r="S29" s="4">
+        <v>1100</v>
+      </c>
+      <c r="T29" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="U29" s="2"/>
+      <c r="V29" s="2"/>
+      <c r="W29" s="2"/>
+      <c r="X29" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y29" s="2"/>
+      <c r="Z29" s="2"/>
+      <c r="AA29" s="2"/>
+      <c r="AB29" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="AC29" s="2"/>
+      <c r="AD29" s="2"/>
+      <c r="AE29" s="2"/>
+      <c r="AF29" s="2"/>
+    </row>
+    <row r="30" spans="1:32">
+      <c r="A30" s="2">
+        <v>20</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="C30" s="4"/>
+      <c r="D30" s="2">
+        <v>1106</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="G30" s="2"/>
+      <c r="H30" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="I30" s="2"/>
+      <c r="J30" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="K30" s="2"/>
+      <c r="L30" s="2"/>
+      <c r="M30" s="2"/>
+      <c r="N30" s="5">
+        <v>3</v>
+      </c>
+      <c r="O30" s="5"/>
+      <c r="P30" s="5"/>
+      <c r="Q30" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="R30" s="5">
+        <v>495</v>
+      </c>
+      <c r="S30" s="4">
+        <v>1485</v>
+      </c>
+      <c r="T30" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="U30" s="2"/>
+      <c r="V30" s="2"/>
+      <c r="W30" s="2"/>
+      <c r="X30" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="Y30" s="2"/>
+      <c r="Z30" s="2"/>
+      <c r="AA30" s="2"/>
+      <c r="AB30" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="AC30" s="2"/>
+      <c r="AD30" s="2"/>
+      <c r="AE30" s="2"/>
+      <c r="AF30" s="2"/>
+    </row>
+    <row r="31" spans="1:32">
+      <c r="A31" s="2">
+        <v>21</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="C31" s="4"/>
+      <c r="D31" s="2">
+        <v>1001</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="F31" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="D26" t="s">
+      <c r="G31" s="2"/>
+      <c r="H31" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="G26" t="s">
+      <c r="I31" s="2"/>
+      <c r="J31" s="2" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="29" spans="1:32">
-      <c r="A29" t="s">
+      <c r="K31" s="2"/>
+      <c r="L31" s="2"/>
+      <c r="M31" s="2"/>
+      <c r="N31" s="5">
+        <v>1</v>
+      </c>
+      <c r="O31" s="5"/>
+      <c r="P31" s="5"/>
+      <c r="Q31" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="D29" t="s">
+      <c r="R31" s="5">
+        <v>29.5</v>
+      </c>
+      <c r="S31" s="4">
+        <v>29.5</v>
+      </c>
+      <c r="T31" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="U31" s="2"/>
+      <c r="V31" s="2"/>
+      <c r="W31" s="2"/>
+      <c r="X31" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y31" s="2"/>
+      <c r="Z31" s="2"/>
+      <c r="AA31" s="2"/>
+      <c r="AB31" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="G29" t="s">
+      <c r="AC31" s="2"/>
+      <c r="AD31" s="2"/>
+      <c r="AE31" s="2"/>
+      <c r="AF31" s="2"/>
+    </row>
+    <row r="32" spans="1:32">
+      <c r="A32" s="2">
+        <v>22</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="C32" s="4"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2" t="s">
         <v>104</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G32" s="2"/>
+      <c r="H32" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="I32" s="2"/>
+      <c r="J32" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="K32" s="2"/>
+      <c r="L32" s="2"/>
+      <c r="M32" s="2"/>
+      <c r="N32" s="5">
+        <v>1</v>
+      </c>
+      <c r="O32" s="5"/>
+      <c r="P32" s="5"/>
+      <c r="Q32" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="R32" s="5">
+        <v>12320</v>
+      </c>
+      <c r="S32" s="4">
+        <v>12320</v>
+      </c>
+      <c r="T32" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="U32" s="2"/>
+      <c r="V32" s="2"/>
+      <c r="W32" s="2"/>
+      <c r="X32" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="Y32" s="2"/>
+      <c r="Z32" s="2"/>
+      <c r="AA32" s="2"/>
+      <c r="AB32" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC32" s="2"/>
+      <c r="AD32" s="2"/>
+      <c r="AE32" s="2"/>
+      <c r="AF32" s="2"/>
+    </row>
+    <row r="33" spans="1:32">
+      <c r="A33" s="2">
+        <v>23</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="C33" s="4"/>
+      <c r="D33" s="2">
+        <v>1016</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="G33" s="2"/>
+      <c r="H33" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="I33" s="2"/>
+      <c r="J33" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="K33" s="2"/>
+      <c r="L33" s="2"/>
+      <c r="M33" s="2"/>
+      <c r="N33" s="5">
+        <v>5</v>
+      </c>
+      <c r="O33" s="5"/>
+      <c r="P33" s="5"/>
+      <c r="Q33" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="R33" s="5">
+        <v>800</v>
+      </c>
+      <c r="S33" s="4">
+        <v>4000</v>
+      </c>
+      <c r="T33" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="U33" s="2"/>
+      <c r="V33" s="2"/>
+      <c r="W33" s="2"/>
+      <c r="X33" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="Y33" s="2"/>
+      <c r="Z33" s="2"/>
+      <c r="AA33" s="2"/>
+      <c r="AB33" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="AC33" s="2"/>
+      <c r="AD33" s="2"/>
+      <c r="AE33" s="2"/>
+      <c r="AF33" s="2"/>
+    </row>
+    <row r="34" spans="1:32">
+      <c r="A34" s="2">
+        <v>24</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="C34" s="4"/>
+      <c r="D34" s="2">
+        <v>1000</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="G34" s="2"/>
+      <c r="H34" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="I34" s="2"/>
+      <c r="J34" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="K34" s="2"/>
+      <c r="L34" s="2"/>
+      <c r="M34" s="2"/>
+      <c r="N34" s="5">
+        <v>1</v>
+      </c>
+      <c r="O34" s="5"/>
+      <c r="P34" s="5"/>
+      <c r="Q34" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="R34" s="5">
+        <v>60</v>
+      </c>
+      <c r="S34" s="4">
+        <v>60</v>
+      </c>
+      <c r="T34" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="U34" s="2"/>
+      <c r="V34" s="2"/>
+      <c r="W34" s="2"/>
+      <c r="X34" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y34" s="2"/>
+      <c r="Z34" s="2"/>
+      <c r="AA34" s="2"/>
+      <c r="AB34" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="AC34" s="2"/>
+      <c r="AD34" s="2"/>
+      <c r="AE34" s="2"/>
+      <c r="AF34" s="2"/>
+    </row>
+    <row r="35" spans="1:32">
+      <c r="A35" s="2">
+        <v>25</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="C35" s="4"/>
+      <c r="D35" s="2">
+        <v>1107</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="G35" s="2"/>
+      <c r="H35" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="I35" s="2"/>
+      <c r="J35" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="K35" s="2"/>
+      <c r="L35" s="2"/>
+      <c r="M35" s="2"/>
+      <c r="N35" s="5">
+        <v>20</v>
+      </c>
+      <c r="O35" s="5"/>
+      <c r="P35" s="5"/>
+      <c r="Q35" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="R35" s="5">
+        <v>34.21</v>
+      </c>
+      <c r="S35" s="4">
+        <v>684.2</v>
+      </c>
+      <c r="T35" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="U35" s="2"/>
+      <c r="V35" s="2"/>
+      <c r="W35" s="2"/>
+      <c r="X35" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="Y35" s="2"/>
+      <c r="Z35" s="2"/>
+      <c r="AA35" s="2"/>
+      <c r="AB35" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="AC35" s="2"/>
+      <c r="AD35" s="2"/>
+      <c r="AE35" s="2"/>
+      <c r="AF35" s="2"/>
+    </row>
+    <row r="36" spans="1:32">
+      <c r="A36" s="2">
+        <v>26</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="C36" s="4"/>
+      <c r="D36" s="2">
+        <v>1016</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="G36" s="2"/>
+      <c r="H36" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="I36" s="2"/>
+      <c r="J36" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="K36" s="2"/>
+      <c r="L36" s="2"/>
+      <c r="M36" s="2"/>
+      <c r="N36" s="5">
+        <v>1</v>
+      </c>
+      <c r="O36" s="5"/>
+      <c r="P36" s="5"/>
+      <c r="Q36" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="R36" s="5">
+        <v>800</v>
+      </c>
+      <c r="S36" s="4">
+        <v>800</v>
+      </c>
+      <c r="T36" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="U36" s="2"/>
+      <c r="V36" s="2"/>
+      <c r="W36" s="2"/>
+      <c r="X36" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="Y36" s="2"/>
+      <c r="Z36" s="2"/>
+      <c r="AA36" s="2"/>
+      <c r="AB36" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="AC36" s="2"/>
+      <c r="AD36" s="2"/>
+      <c r="AE36" s="2"/>
+      <c r="AF36" s="2"/>
+    </row>
+    <row r="37" spans="1:32">
+      <c r="A37" s="2">
+        <v>27</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="C37" s="4"/>
+      <c r="D37" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="F37" s="2"/>
+      <c r="G37" s="2"/>
+      <c r="H37" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="I37" s="2"/>
+      <c r="J37" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="K37" s="2"/>
+      <c r="L37" s="2"/>
+      <c r="M37" s="2"/>
+      <c r="N37" s="5">
+        <v>10</v>
+      </c>
+      <c r="O37" s="5"/>
+      <c r="P37" s="5"/>
+      <c r="Q37" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="R37" s="5">
+        <v>11</v>
+      </c>
+      <c r="S37" s="4">
+        <v>110</v>
+      </c>
+      <c r="T37" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="U37" s="2"/>
+      <c r="V37" s="2"/>
+      <c r="W37" s="2"/>
+      <c r="X37" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="Y37" s="2"/>
+      <c r="Z37" s="2"/>
+      <c r="AA37" s="2"/>
+      <c r="AB37" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="AC37" s="2"/>
+      <c r="AD37" s="2"/>
+      <c r="AE37" s="2"/>
+      <c r="AF37" s="2"/>
+    </row>
+    <row r="38" spans="1:32">
+      <c r="A38" s="2">
+        <v>28</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="C38" s="4"/>
+      <c r="D38" s="2">
+        <v>1015</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="G38" s="2"/>
+      <c r="H38" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="I38" s="2"/>
+      <c r="J38" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="K38" s="2"/>
+      <c r="L38" s="2"/>
+      <c r="M38" s="2"/>
+      <c r="N38" s="5">
+        <v>6</v>
+      </c>
+      <c r="O38" s="5"/>
+      <c r="P38" s="5"/>
+      <c r="Q38" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="R38" s="5">
+        <v>610</v>
+      </c>
+      <c r="S38" s="4">
+        <v>3660</v>
+      </c>
+      <c r="T38" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="U38" s="2"/>
+      <c r="V38" s="2"/>
+      <c r="W38" s="2"/>
+      <c r="X38" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="Y38" s="2"/>
+      <c r="Z38" s="2"/>
+      <c r="AA38" s="2"/>
+      <c r="AB38" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="AC38" s="2"/>
+      <c r="AD38" s="2"/>
+      <c r="AE38" s="2"/>
+      <c r="AF38" s="2"/>
+    </row>
+    <row r="39" spans="1:32">
+      <c r="A39" s="2">
+        <v>29</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="C39" s="4"/>
+      <c r="D39" s="2">
+        <v>1015</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="G39" s="2"/>
+      <c r="H39" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="I39" s="2"/>
+      <c r="J39" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="K39" s="2"/>
+      <c r="L39" s="2"/>
+      <c r="M39" s="2"/>
+      <c r="N39" s="5">
+        <v>3</v>
+      </c>
+      <c r="O39" s="5"/>
+      <c r="P39" s="5"/>
+      <c r="Q39" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="R39" s="5">
+        <v>750</v>
+      </c>
+      <c r="S39" s="4">
+        <v>2250</v>
+      </c>
+      <c r="T39" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="U39" s="2"/>
+      <c r="V39" s="2"/>
+      <c r="W39" s="2"/>
+      <c r="X39" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="Y39" s="2"/>
+      <c r="Z39" s="2"/>
+      <c r="AA39" s="2"/>
+      <c r="AB39" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="AC39" s="2"/>
+      <c r="AD39" s="2"/>
+      <c r="AE39" s="2"/>
+      <c r="AF39" s="2"/>
+    </row>
+    <row r="40" spans="1:32">
+      <c r="A40" s="2">
+        <v>30</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="C40" s="4"/>
+      <c r="D40" s="2">
+        <v>1015</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="G40" s="2"/>
+      <c r="H40" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="I40" s="2"/>
+      <c r="J40" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="K40" s="2"/>
+      <c r="L40" s="2"/>
+      <c r="M40" s="2"/>
+      <c r="N40" s="5">
+        <v>3</v>
+      </c>
+      <c r="O40" s="5"/>
+      <c r="P40" s="5"/>
+      <c r="Q40" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="R40" s="5">
+        <v>750</v>
+      </c>
+      <c r="S40" s="4">
+        <v>2250</v>
+      </c>
+      <c r="T40" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="U40" s="2"/>
+      <c r="V40" s="2"/>
+      <c r="W40" s="2"/>
+      <c r="X40" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="Y40" s="2"/>
+      <c r="Z40" s="2"/>
+      <c r="AA40" s="2"/>
+      <c r="AB40" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="AC40" s="2"/>
+      <c r="AD40" s="2"/>
+      <c r="AE40" s="2"/>
+      <c r="AF40" s="2"/>
+    </row>
+    <row r="41" spans="1:32">
+      <c r="A41" s="2">
+        <v>31</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="C41" s="4"/>
+      <c r="D41" s="2">
+        <v>1042</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G41" s="2"/>
+      <c r="H41" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="I41" s="2"/>
+      <c r="J41" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="K41" s="2"/>
+      <c r="L41" s="2"/>
+      <c r="M41" s="2"/>
+      <c r="N41" s="5">
+        <v>5</v>
+      </c>
+      <c r="O41" s="5"/>
+      <c r="P41" s="5"/>
+      <c r="Q41" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="R41" s="5">
+        <v>12.7</v>
+      </c>
+      <c r="S41" s="4">
+        <v>63.5</v>
+      </c>
+      <c r="T41" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="U41" s="2"/>
+      <c r="V41" s="2"/>
+      <c r="W41" s="2"/>
+      <c r="X41" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="Y41" s="2"/>
+      <c r="Z41" s="2"/>
+      <c r="AA41" s="2"/>
+      <c r="AB41" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="AC41" s="2"/>
+      <c r="AD41" s="2"/>
+      <c r="AE41" s="2"/>
+      <c r="AF41" s="2"/>
+    </row>
+    <row r="42" spans="1:32">
+      <c r="A42" s="2">
+        <v>32</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="C42" s="4"/>
+      <c r="D42" s="2">
+        <v>31</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="G42" s="2"/>
+      <c r="H42" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="I42" s="2"/>
+      <c r="J42" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="K42" s="2"/>
+      <c r="L42" s="2"/>
+      <c r="M42" s="2"/>
+      <c r="N42" s="5">
+        <v>1</v>
+      </c>
+      <c r="O42" s="5"/>
+      <c r="P42" s="5"/>
+      <c r="Q42" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="R42" s="5">
+        <v>85</v>
+      </c>
+      <c r="S42" s="4">
+        <v>85</v>
+      </c>
+      <c r="T42" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="U42" s="2"/>
+      <c r="V42" s="2"/>
+      <c r="W42" s="2"/>
+      <c r="X42" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="Y42" s="2"/>
+      <c r="Z42" s="2"/>
+      <c r="AA42" s="2"/>
+      <c r="AB42" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="AC42" s="2"/>
+      <c r="AD42" s="2"/>
+      <c r="AE42" s="2"/>
+      <c r="AF42" s="2"/>
+    </row>
+    <row r="43" spans="1:32">
+      <c r="A43" s="2">
+        <v>33</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="C43" s="4"/>
+      <c r="D43" s="2">
+        <v>1017</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="F43" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="G43" s="2"/>
+      <c r="H43" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="I43" s="2"/>
+      <c r="J43" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="K43" s="2"/>
+      <c r="L43" s="2"/>
+      <c r="M43" s="2"/>
+      <c r="N43" s="5">
+        <v>1</v>
+      </c>
+      <c r="O43" s="5"/>
+      <c r="P43" s="5"/>
+      <c r="Q43" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="R43" s="5">
+        <v>700</v>
+      </c>
+      <c r="S43" s="4">
+        <v>700</v>
+      </c>
+      <c r="T43" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="U43" s="2"/>
+      <c r="V43" s="2"/>
+      <c r="W43" s="2"/>
+      <c r="X43" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y43" s="2"/>
+      <c r="Z43" s="2"/>
+      <c r="AA43" s="2"/>
+      <c r="AB43" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="AC43" s="2"/>
+      <c r="AD43" s="2"/>
+      <c r="AE43" s="2"/>
+      <c r="AF43" s="2"/>
+    </row>
+    <row r="44" spans="1:32">
+      <c r="A44" s="2">
+        <v>34</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="C44" s="4"/>
+      <c r="D44" s="2">
+        <v>1000</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="G44" s="2"/>
+      <c r="H44" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="I44" s="2"/>
+      <c r="J44" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="K44" s="2"/>
+      <c r="L44" s="2"/>
+      <c r="M44" s="2"/>
+      <c r="N44" s="5">
+        <v>1</v>
+      </c>
+      <c r="O44" s="5"/>
+      <c r="P44" s="5"/>
+      <c r="Q44" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="R44" s="5">
+        <v>30</v>
+      </c>
+      <c r="S44" s="4">
+        <v>30</v>
+      </c>
+      <c r="T44" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="U44" s="2"/>
+      <c r="V44" s="2"/>
+      <c r="W44" s="2"/>
+      <c r="X44" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="Y44" s="2"/>
+      <c r="Z44" s="2"/>
+      <c r="AA44" s="2"/>
+      <c r="AB44" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="AC44" s="2"/>
+      <c r="AD44" s="2"/>
+      <c r="AE44" s="2"/>
+      <c r="AF44" s="2"/>
+    </row>
+    <row r="45" spans="1:32">
+      <c r="A45" s="2">
+        <v>35</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="C45" s="4"/>
+      <c r="D45" s="2">
+        <v>1108</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="F45" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="G45" s="2"/>
+      <c r="H45" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="I45" s="2"/>
+      <c r="J45" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="K45" s="2"/>
+      <c r="L45" s="2"/>
+      <c r="M45" s="2"/>
+      <c r="N45" s="5">
+        <v>20</v>
+      </c>
+      <c r="O45" s="5"/>
+      <c r="P45" s="5"/>
+      <c r="Q45" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="R45" s="5">
+        <v>34.95</v>
+      </c>
+      <c r="S45" s="4">
+        <v>699</v>
+      </c>
+      <c r="T45" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="U45" s="2"/>
+      <c r="V45" s="2"/>
+      <c r="W45" s="2"/>
+      <c r="X45" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="Y45" s="2"/>
+      <c r="Z45" s="2"/>
+      <c r="AA45" s="2"/>
+      <c r="AB45" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="AC45" s="2"/>
+      <c r="AD45" s="2"/>
+      <c r="AE45" s="2"/>
+      <c r="AF45" s="2"/>
+    </row>
+    <row r="46" spans="1:32">
+      <c r="A46" s="2">
+        <v>36</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="C46" s="4"/>
+      <c r="D46" s="2">
+        <v>1096</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="F46" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="G46" s="2"/>
+      <c r="H46" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="I46" s="2"/>
+      <c r="J46" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="K46" s="2"/>
+      <c r="L46" s="2"/>
+      <c r="M46" s="2"/>
+      <c r="N46" s="5">
+        <v>22</v>
+      </c>
+      <c r="O46" s="5"/>
+      <c r="P46" s="5"/>
+      <c r="Q46" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="R46" s="5">
+        <v>11.45</v>
+      </c>
+      <c r="S46" s="4">
+        <v>251.9</v>
+      </c>
+      <c r="T46" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="U46" s="2"/>
+      <c r="V46" s="2"/>
+      <c r="W46" s="2"/>
+      <c r="X46" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="Y46" s="2"/>
+      <c r="Z46" s="2"/>
+      <c r="AA46" s="2"/>
+      <c r="AB46" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="AC46" s="2"/>
+      <c r="AD46" s="2"/>
+      <c r="AE46" s="2"/>
+      <c r="AF46" s="2"/>
+    </row>
+    <row r="47" spans="1:32">
+      <c r="A47" s="2">
+        <v>37</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="C47" s="4"/>
+      <c r="D47" s="2">
+        <v>1095</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="F47" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="G47" s="2"/>
+      <c r="H47" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="I47" s="2"/>
+      <c r="J47" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="K47" s="2"/>
+      <c r="L47" s="2"/>
+      <c r="M47" s="2"/>
+      <c r="N47" s="5">
+        <v>2</v>
+      </c>
+      <c r="O47" s="5"/>
+      <c r="P47" s="5"/>
+      <c r="Q47" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="R47" s="5">
+        <v>341</v>
+      </c>
+      <c r="S47" s="4">
+        <v>682</v>
+      </c>
+      <c r="T47" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="U47" s="2"/>
+      <c r="V47" s="2"/>
+      <c r="W47" s="2"/>
+      <c r="X47" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="Y47" s="2"/>
+      <c r="Z47" s="2"/>
+      <c r="AA47" s="2"/>
+      <c r="AB47" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="AC47" s="2"/>
+      <c r="AD47" s="2"/>
+      <c r="AE47" s="2"/>
+      <c r="AF47" s="2"/>
+    </row>
+    <row r="48" spans="1:32">
+      <c r="A48" s="2">
+        <v>38</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="C48" s="4"/>
+      <c r="D48" s="2">
+        <v>1108</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="F48" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="G48" s="2"/>
+      <c r="H48" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="I48" s="2"/>
+      <c r="J48" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="K48" s="2"/>
+      <c r="L48" s="2"/>
+      <c r="M48" s="2"/>
+      <c r="N48" s="5">
+        <v>36</v>
+      </c>
+      <c r="O48" s="5"/>
+      <c r="P48" s="5"/>
+      <c r="Q48" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="R48" s="5">
+        <v>34.95</v>
+      </c>
+      <c r="S48" s="4">
+        <v>1258.2</v>
+      </c>
+      <c r="T48" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="U48" s="2"/>
+      <c r="V48" s="2"/>
+      <c r="W48" s="2"/>
+      <c r="X48" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="Y48" s="2"/>
+      <c r="Z48" s="2"/>
+      <c r="AA48" s="2"/>
+      <c r="AB48" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="AC48" s="2"/>
+      <c r="AD48" s="2"/>
+      <c r="AE48" s="2"/>
+      <c r="AF48" s="2"/>
+    </row>
+    <row r="49" spans="1:32">
+      <c r="A49" s="2">
+        <v>39</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="C49" s="4"/>
+      <c r="D49" s="2"/>
+      <c r="E49" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="F49" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G49" s="2"/>
+      <c r="H49" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="I49" s="2"/>
+      <c r="J49" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="K49" s="2"/>
+      <c r="L49" s="2"/>
+      <c r="M49" s="2"/>
+      <c r="N49" s="5">
+        <v>1</v>
+      </c>
+      <c r="O49" s="5"/>
+      <c r="P49" s="5"/>
+      <c r="Q49" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="R49" s="5">
+        <v>0</v>
+      </c>
+      <c r="S49" s="4">
+        <v>0</v>
+      </c>
+      <c r="T49" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="U49" s="2"/>
+      <c r="V49" s="2"/>
+      <c r="W49" s="2"/>
+      <c r="X49" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y49" s="2"/>
+      <c r="Z49" s="2"/>
+      <c r="AA49" s="2"/>
+      <c r="AB49" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="AC49" s="2"/>
+      <c r="AD49" s="2"/>
+      <c r="AE49" s="2"/>
+      <c r="AF49" s="2"/>
+    </row>
+    <row r="50" spans="1:32">
+      <c r="A50" s="2">
+        <v>40</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="C50" s="4"/>
+      <c r="D50" s="2">
+        <v>1096</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="F50" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="G50" s="2"/>
+      <c r="H50" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="I50" s="2"/>
+      <c r="J50" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="K50" s="2"/>
+      <c r="L50" s="2"/>
+      <c r="M50" s="2"/>
+      <c r="N50" s="5">
+        <v>15</v>
+      </c>
+      <c r="O50" s="5"/>
+      <c r="P50" s="5"/>
+      <c r="Q50" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="R50" s="5">
+        <v>11.45</v>
+      </c>
+      <c r="S50" s="4">
+        <v>171.75</v>
+      </c>
+      <c r="T50" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="U50" s="2"/>
+      <c r="V50" s="2"/>
+      <c r="W50" s="2"/>
+      <c r="X50" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="Y50" s="2"/>
+      <c r="Z50" s="2"/>
+      <c r="AA50" s="2"/>
+      <c r="AB50" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="AC50" s="2"/>
+      <c r="AD50" s="2"/>
+      <c r="AE50" s="2"/>
+      <c r="AF50" s="2"/>
+    </row>
+    <row r="51" spans="1:32">
+      <c r="A51" s="2">
+        <v>41</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="C51" s="4"/>
+      <c r="D51" s="2">
+        <v>1073</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="F51" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="G51" s="2"/>
+      <c r="H51" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="I51" s="2"/>
+      <c r="J51" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="K51" s="2"/>
+      <c r="L51" s="2"/>
+      <c r="M51" s="2"/>
+      <c r="N51" s="5">
+        <v>1</v>
+      </c>
+      <c r="O51" s="5"/>
+      <c r="P51" s="5"/>
+      <c r="Q51" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="R51" s="5">
+        <v>280</v>
+      </c>
+      <c r="S51" s="4">
+        <v>280</v>
+      </c>
+      <c r="T51" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="U51" s="2"/>
+      <c r="V51" s="2"/>
+      <c r="W51" s="2"/>
+      <c r="X51" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="Y51" s="2"/>
+      <c r="Z51" s="2"/>
+      <c r="AA51" s="2"/>
+      <c r="AB51" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="AC51" s="2"/>
+      <c r="AD51" s="2"/>
+      <c r="AE51" s="2"/>
+      <c r="AF51" s="2"/>
+    </row>
+    <row r="52" spans="1:32">
+      <c r="A52" s="2">
+        <v>42</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="C52" s="4"/>
+      <c r="D52" s="2"/>
+      <c r="E52" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="F52" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G52" s="2"/>
+      <c r="H52" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="I52" s="2"/>
+      <c r="J52" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="K52" s="2"/>
+      <c r="L52" s="2"/>
+      <c r="M52" s="2"/>
+      <c r="N52" s="5">
+        <v>20</v>
+      </c>
+      <c r="O52" s="5"/>
+      <c r="P52" s="5"/>
+      <c r="Q52" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="R52" s="5">
+        <v>14</v>
+      </c>
+      <c r="S52" s="4">
+        <v>280</v>
+      </c>
+      <c r="T52" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="U52" s="2"/>
+      <c r="V52" s="2"/>
+      <c r="W52" s="2"/>
+      <c r="X52" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="Y52" s="2"/>
+      <c r="Z52" s="2"/>
+      <c r="AA52" s="2"/>
+      <c r="AB52" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="AC52" s="2"/>
+      <c r="AD52" s="2"/>
+      <c r="AE52" s="2"/>
+      <c r="AF52" s="2"/>
+    </row>
+    <row r="53" spans="1:32">
+      <c r="A53" s="2">
+        <v>43</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="C53" s="4"/>
+      <c r="D53" s="2">
+        <v>1075</v>
+      </c>
+      <c r="E53" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="F53" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="G53" s="2"/>
+      <c r="H53" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="I53" s="2"/>
+      <c r="J53" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="K53" s="2"/>
+      <c r="L53" s="2"/>
+      <c r="M53" s="2"/>
+      <c r="N53" s="5">
+        <v>10</v>
+      </c>
+      <c r="O53" s="5"/>
+      <c r="P53" s="5"/>
+      <c r="Q53" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="R53" s="5">
+        <v>7</v>
+      </c>
+      <c r="S53" s="4">
+        <v>70</v>
+      </c>
+      <c r="T53" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="U53" s="2"/>
+      <c r="V53" s="2"/>
+      <c r="W53" s="2"/>
+      <c r="X53" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="Y53" s="2"/>
+      <c r="Z53" s="2"/>
+      <c r="AA53" s="2"/>
+      <c r="AB53" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="AC53" s="2"/>
+      <c r="AD53" s="2"/>
+      <c r="AE53" s="2"/>
+      <c r="AF53" s="2"/>
+    </row>
+    <row r="54" spans="1:32">
+      <c r="A54" s="2">
+        <v>44</v>
+      </c>
+      <c r="B54" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="C54" s="4"/>
+      <c r="D54" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="E54" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="F54" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G54" s="2"/>
+      <c r="H54" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="I54" s="2"/>
+      <c r="J54" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="K54" s="2"/>
+      <c r="L54" s="2"/>
+      <c r="M54" s="2"/>
+      <c r="N54" s="5">
+        <v>2</v>
+      </c>
+      <c r="O54" s="5"/>
+      <c r="P54" s="5"/>
+      <c r="Q54" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="R54" s="5">
+        <v>110</v>
+      </c>
+      <c r="S54" s="4">
+        <v>220</v>
+      </c>
+      <c r="T54" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="U54" s="2"/>
+      <c r="V54" s="2"/>
+      <c r="W54" s="2"/>
+      <c r="X54" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="Y54" s="2"/>
+      <c r="Z54" s="2"/>
+      <c r="AA54" s="2"/>
+      <c r="AB54" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="AC54" s="2"/>
+      <c r="AD54" s="2"/>
+      <c r="AE54" s="2"/>
+      <c r="AF54" s="2"/>
+    </row>
+    <row r="55" spans="1:32">
+      <c r="A55" s="2">
+        <v>45</v>
+      </c>
+      <c r="B55" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="C55" s="4"/>
+      <c r="D55" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="E55" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="F55" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G55" s="2"/>
+      <c r="H55" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="I55" s="2"/>
+      <c r="J55" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="K55" s="2"/>
+      <c r="L55" s="2"/>
+      <c r="M55" s="2"/>
+      <c r="N55" s="5">
+        <v>5</v>
+      </c>
+      <c r="O55" s="5"/>
+      <c r="P55" s="5"/>
+      <c r="Q55" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="R55" s="5">
+        <v>11</v>
+      </c>
+      <c r="S55" s="4">
+        <v>55</v>
+      </c>
+      <c r="T55" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="U55" s="2"/>
+      <c r="V55" s="2"/>
+      <c r="W55" s="2"/>
+      <c r="X55" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="Y55" s="2"/>
+      <c r="Z55" s="2"/>
+      <c r="AA55" s="2"/>
+      <c r="AB55" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="AC55" s="2"/>
+      <c r="AD55" s="2"/>
+      <c r="AE55" s="2"/>
+      <c r="AF55" s="2"/>
+    </row>
+    <row r="56" spans="1:32">
+      <c r="A56" s="2">
+        <v>46</v>
+      </c>
+      <c r="B56" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="C56" s="4"/>
+      <c r="D56" s="2">
+        <v>1007</v>
+      </c>
+      <c r="E56" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="F56" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="G56" s="2"/>
+      <c r="H56" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="I56" s="2"/>
+      <c r="J56" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="K56" s="2"/>
+      <c r="L56" s="2"/>
+      <c r="M56" s="2"/>
+      <c r="N56" s="5">
+        <v>1</v>
+      </c>
+      <c r="O56" s="5"/>
+      <c r="P56" s="5"/>
+      <c r="Q56" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="R56" s="5">
+        <v>4</v>
+      </c>
+      <c r="S56" s="4">
+        <v>4</v>
+      </c>
+      <c r="T56" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="U56" s="2"/>
+      <c r="V56" s="2"/>
+      <c r="W56" s="2"/>
+      <c r="X56" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="Y56" s="2"/>
+      <c r="Z56" s="2"/>
+      <c r="AA56" s="2"/>
+      <c r="AB56" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="AC56" s="2"/>
+      <c r="AD56" s="2"/>
+      <c r="AE56" s="2"/>
+      <c r="AF56" s="2"/>
+    </row>
+    <row r="57" spans="1:32">
+      <c r="A57" s="2">
+        <v>47</v>
+      </c>
+      <c r="B57" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="C57" s="4"/>
+      <c r="D57" s="2"/>
+      <c r="E57" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="F57" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G57" s="2"/>
+      <c r="H57" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="I57" s="2"/>
+      <c r="J57" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="K57" s="2"/>
+      <c r="L57" s="2"/>
+      <c r="M57" s="2"/>
+      <c r="N57" s="5">
+        <v>20</v>
+      </c>
+      <c r="O57" s="5"/>
+      <c r="P57" s="5"/>
+      <c r="Q57" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="R57" s="5">
+        <v>14</v>
+      </c>
+      <c r="S57" s="4">
+        <v>280</v>
+      </c>
+      <c r="T57" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="U57" s="2"/>
+      <c r="V57" s="2"/>
+      <c r="W57" s="2"/>
+      <c r="X57" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="Y57" s="2"/>
+      <c r="Z57" s="2"/>
+      <c r="AA57" s="2"/>
+      <c r="AB57" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="AC57" s="2"/>
+      <c r="AD57" s="2"/>
+      <c r="AE57" s="2"/>
+      <c r="AF57" s="2"/>
+    </row>
+    <row r="58" spans="1:32">
+      <c r="A58" s="2">
+        <v>48</v>
+      </c>
+      <c r="B58" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="C58" s="4"/>
+      <c r="D58" s="2">
+        <v>1096</v>
+      </c>
+      <c r="E58" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="F58" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="G58" s="2"/>
+      <c r="H58" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="I58" s="2"/>
+      <c r="J58" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="K58" s="2"/>
+      <c r="L58" s="2"/>
+      <c r="M58" s="2"/>
+      <c r="N58" s="5">
+        <v>11</v>
+      </c>
+      <c r="O58" s="5"/>
+      <c r="P58" s="5"/>
+      <c r="Q58" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="R58" s="5">
+        <v>11.45</v>
+      </c>
+      <c r="S58" s="4">
+        <v>125.95</v>
+      </c>
+      <c r="T58" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="U58" s="2"/>
+      <c r="V58" s="2"/>
+      <c r="W58" s="2"/>
+      <c r="X58" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="Y58" s="2"/>
+      <c r="Z58" s="2"/>
+      <c r="AA58" s="2"/>
+      <c r="AB58" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="AC58" s="2"/>
+      <c r="AD58" s="2"/>
+      <c r="AE58" s="2"/>
+      <c r="AF58" s="2"/>
+    </row>
+    <row r="59" spans="1:32">
+      <c r="A59" s="2">
+        <v>49</v>
+      </c>
+      <c r="B59" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="C59" s="4"/>
+      <c r="D59" s="2">
+        <v>1101</v>
+      </c>
+      <c r="E59" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="F59" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="G59" s="2"/>
+      <c r="H59" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="I59" s="2"/>
+      <c r="J59" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="K59" s="2"/>
+      <c r="L59" s="2"/>
+      <c r="M59" s="2"/>
+      <c r="N59" s="5">
+        <v>3</v>
+      </c>
+      <c r="O59" s="5"/>
+      <c r="P59" s="5"/>
+      <c r="Q59" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="R59" s="5">
+        <v>50</v>
+      </c>
+      <c r="S59" s="4">
+        <v>150</v>
+      </c>
+      <c r="T59" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="U59" s="2"/>
+      <c r="V59" s="2"/>
+      <c r="W59" s="2"/>
+      <c r="X59" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="Y59" s="2"/>
+      <c r="Z59" s="2"/>
+      <c r="AA59" s="2"/>
+      <c r="AB59" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="AC59" s="2"/>
+      <c r="AD59" s="2"/>
+      <c r="AE59" s="2"/>
+      <c r="AF59" s="2"/>
+    </row>
+    <row r="60" spans="1:32">
+      <c r="B60" s="3"/>
+      <c r="C60" s="3"/>
+      <c r="F60"/>
+      <c r="G60"/>
+      <c r="H60"/>
+      <c r="I60"/>
+      <c r="J60"/>
+      <c r="K60"/>
+      <c r="L60"/>
+      <c r="M60"/>
+      <c r="N60" s="3"/>
+      <c r="O60" s="3"/>
+      <c r="P60" s="3"/>
+      <c r="Q60" s="3"/>
+      <c r="R60" s="3"/>
+      <c r="S60" s="3"/>
+      <c r="T60"/>
+      <c r="U60"/>
+      <c r="V60"/>
+      <c r="W60"/>
+      <c r="X60"/>
+      <c r="Y60"/>
+      <c r="Z60"/>
+      <c r="AA60"/>
+      <c r="AB60"/>
+      <c r="AC60"/>
+      <c r="AD60"/>
+      <c r="AE60"/>
+    </row>
+    <row r="62" spans="1:32">
+      <c r="A62" t="s">
+        <v>184</v>
+      </c>
+      <c r="D62" t="s">
+        <v>185</v>
+      </c>
+      <c r="G62" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="65" spans="1:32">
+      <c r="A65" t="s">
+        <v>187</v>
+      </c>
+      <c r="D65" t="s">
+        <v>188</v>
+      </c>
+      <c r="G65" t="s">
+        <v>189</v>
       </c>
     </row>
   </sheetData>
@@ -2007,8 +4434,44 @@
     <protectedRange name="pb3afbace8f6f7f6354d93ecb3a9b663f" sqref="A21:AF21" password="C724"/>
     <protectedRange name="p541e80c77299ba74bfe0a8ca3ee9141d" sqref="A22:AF22" password="C724"/>
     <protectedRange name="p23fee5e85d52e11b1d93f70d48585c2b" sqref="A23:AF23" password="C724"/>
-    <protectedRange name="p9f36a12064855111794ae27561c69276" sqref="A26:AC26" password="C724"/>
-    <protectedRange name="p807bd27742240b7001ab7b50e6be40d4" sqref="A28:AC28" password="C724"/>
+    <protectedRange name="pa1cabf18dd71e2ef9a7afeb8defea173" sqref="A24:AF24" password="C724"/>
+    <protectedRange name="p9653d8192543ed2e4821e86ac5e7c48d" sqref="A25:AF25" password="C724"/>
+    <protectedRange name="p62793a4b2b351f0f6ab2c6179fb2e5f1" sqref="A26:AF26" password="C724"/>
+    <protectedRange name="p58b5cbb444cefa90d8ef0c866d17540b" sqref="A27:AF27" password="C724"/>
+    <protectedRange name="p0c030d21cdba4738ec834274cf7504e5" sqref="A28:AF28" password="C724"/>
+    <protectedRange name="p3412205006155e0ea7b21c9392c6de5e" sqref="A29:AF29" password="C724"/>
+    <protectedRange name="pcbb41e46e5ff7c5f2e714f24d6747826" sqref="A30:AF30" password="C724"/>
+    <protectedRange name="p51db9f918d7d27f58e588d0abaeaac83" sqref="A31:AF31" password="C724"/>
+    <protectedRange name="p59f169197112919b2345e38ec768a5fd" sqref="A32:AF32" password="C724"/>
+    <protectedRange name="p13480379ab0779265c41ae7a6039c0f3" sqref="A33:AF33" password="C724"/>
+    <protectedRange name="pbb722cb123e435ef217c42081889ee15" sqref="A34:AF34" password="C724"/>
+    <protectedRange name="p3959ed0c5de07b3fc43cf98f8c516cd3" sqref="A35:AF35" password="C724"/>
+    <protectedRange name="p2751352752bfd688bccda91fe1482587" sqref="A36:AF36" password="C724"/>
+    <protectedRange name="p2843a14aa55e1e88631c3dfdad51a96a" sqref="A37:AF37" password="C724"/>
+    <protectedRange name="p12e05302b62cfbb94cf09a87d54db31e" sqref="A38:AF38" password="C724"/>
+    <protectedRange name="peca44db6a1ee5a4d4bcb9cbbdcfbd0b8" sqref="A39:AF39" password="C724"/>
+    <protectedRange name="pa6d5b4255f502ecf47fcaae63f5deb28" sqref="A40:AF40" password="C724"/>
+    <protectedRange name="pf1af4a1c4bfc2c38e56aaf3ce6a2edc1" sqref="A41:AF41" password="C724"/>
+    <protectedRange name="p95c2e5c28d6f6f561eb914f95f638828" sqref="A42:AF42" password="C724"/>
+    <protectedRange name="p111d7a1d128fb8383c27971e19e5d05f" sqref="A43:AF43" password="C724"/>
+    <protectedRange name="p1c0b9d16d1dd70368e5f9895d70af994" sqref="A44:AF44" password="C724"/>
+    <protectedRange name="p25c42e7b990f3edaa8fab0f33ca44908" sqref="A45:AF45" password="C724"/>
+    <protectedRange name="p2f789aa2a54920673a050559244ec11c" sqref="A46:AF46" password="C724"/>
+    <protectedRange name="p87a2b6cddf95b5cc2defb9ff0bb538cd" sqref="A47:AF47" password="C724"/>
+    <protectedRange name="pec85682b91756a8981cd7a16de90e6b7" sqref="A48:AF48" password="C724"/>
+    <protectedRange name="pbfbdda082f0815ecc119a9b22600e393" sqref="A49:AF49" password="C724"/>
+    <protectedRange name="pd8c7cb5a552f6a83056c8b5aca602418" sqref="A50:AF50" password="C724"/>
+    <protectedRange name="p72d28872b6d3888b71f759ec1e39769f" sqref="A51:AF51" password="C724"/>
+    <protectedRange name="p9ba3299d77acbae879891a6d41a03c33" sqref="A52:AF52" password="C724"/>
+    <protectedRange name="p3ae9ab9a7647470a7fdf87951bc0dd1e" sqref="A53:AF53" password="C724"/>
+    <protectedRange name="p51cca0cfeb28fae64091b18942cdc49d" sqref="A54:AF54" password="C724"/>
+    <protectedRange name="p6c85cc7f739e4372bd79c8dc986addff" sqref="A55:AF55" password="C724"/>
+    <protectedRange name="p0fa845334db398a23a2ffe23724a1d93" sqref="A56:AF56" password="C724"/>
+    <protectedRange name="p2cccefc299a9da824d33bee77d009c25" sqref="A57:AF57" password="C724"/>
+    <protectedRange name="p663896ebb3af5cdb38a84d9f674dab12" sqref="A58:AF58" password="C724"/>
+    <protectedRange name="p63739023b198c22000699ad32e160c5c" sqref="A59:AF59" password="C724"/>
+    <protectedRange name="p95365a24e85f63181f15105c7b8bb3f9" sqref="A62:AC62" password="C724"/>
+    <protectedRange name="p61ee90d5d0553e35b8314681af9dea32" sqref="A64:AC64" password="C724"/>
   </protectedRanges>
   <mergeCells>
     <mergeCell ref="B11:C11"/>
@@ -2123,6 +4586,294 @@
     <mergeCell ref="T24:W24"/>
     <mergeCell ref="X24:AA24"/>
     <mergeCell ref="AB24:AE24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="J25:M25"/>
+    <mergeCell ref="N25:P25"/>
+    <mergeCell ref="T25:W25"/>
+    <mergeCell ref="X25:AA25"/>
+    <mergeCell ref="AB25:AE25"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="F26:G26"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="J26:M26"/>
+    <mergeCell ref="N26:P26"/>
+    <mergeCell ref="T26:W26"/>
+    <mergeCell ref="X26:AA26"/>
+    <mergeCell ref="AB26:AE26"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="J27:M27"/>
+    <mergeCell ref="N27:P27"/>
+    <mergeCell ref="T27:W27"/>
+    <mergeCell ref="X27:AA27"/>
+    <mergeCell ref="AB27:AE27"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="J28:M28"/>
+    <mergeCell ref="N28:P28"/>
+    <mergeCell ref="T28:W28"/>
+    <mergeCell ref="X28:AA28"/>
+    <mergeCell ref="AB28:AE28"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="H29:I29"/>
+    <mergeCell ref="J29:M29"/>
+    <mergeCell ref="N29:P29"/>
+    <mergeCell ref="T29:W29"/>
+    <mergeCell ref="X29:AA29"/>
+    <mergeCell ref="AB29:AE29"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="H30:I30"/>
+    <mergeCell ref="J30:M30"/>
+    <mergeCell ref="N30:P30"/>
+    <mergeCell ref="T30:W30"/>
+    <mergeCell ref="X30:AA30"/>
+    <mergeCell ref="AB30:AE30"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="F31:G31"/>
+    <mergeCell ref="H31:I31"/>
+    <mergeCell ref="J31:M31"/>
+    <mergeCell ref="N31:P31"/>
+    <mergeCell ref="T31:W31"/>
+    <mergeCell ref="X31:AA31"/>
+    <mergeCell ref="AB31:AE31"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="F32:G32"/>
+    <mergeCell ref="H32:I32"/>
+    <mergeCell ref="J32:M32"/>
+    <mergeCell ref="N32:P32"/>
+    <mergeCell ref="T32:W32"/>
+    <mergeCell ref="X32:AA32"/>
+    <mergeCell ref="AB32:AE32"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="F33:G33"/>
+    <mergeCell ref="H33:I33"/>
+    <mergeCell ref="J33:M33"/>
+    <mergeCell ref="N33:P33"/>
+    <mergeCell ref="T33:W33"/>
+    <mergeCell ref="X33:AA33"/>
+    <mergeCell ref="AB33:AE33"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="F34:G34"/>
+    <mergeCell ref="H34:I34"/>
+    <mergeCell ref="J34:M34"/>
+    <mergeCell ref="N34:P34"/>
+    <mergeCell ref="T34:W34"/>
+    <mergeCell ref="X34:AA34"/>
+    <mergeCell ref="AB34:AE34"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="F35:G35"/>
+    <mergeCell ref="H35:I35"/>
+    <mergeCell ref="J35:M35"/>
+    <mergeCell ref="N35:P35"/>
+    <mergeCell ref="T35:W35"/>
+    <mergeCell ref="X35:AA35"/>
+    <mergeCell ref="AB35:AE35"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="F36:G36"/>
+    <mergeCell ref="H36:I36"/>
+    <mergeCell ref="J36:M36"/>
+    <mergeCell ref="N36:P36"/>
+    <mergeCell ref="T36:W36"/>
+    <mergeCell ref="X36:AA36"/>
+    <mergeCell ref="AB36:AE36"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="F37:G37"/>
+    <mergeCell ref="H37:I37"/>
+    <mergeCell ref="J37:M37"/>
+    <mergeCell ref="N37:P37"/>
+    <mergeCell ref="T37:W37"/>
+    <mergeCell ref="X37:AA37"/>
+    <mergeCell ref="AB37:AE37"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="F38:G38"/>
+    <mergeCell ref="H38:I38"/>
+    <mergeCell ref="J38:M38"/>
+    <mergeCell ref="N38:P38"/>
+    <mergeCell ref="T38:W38"/>
+    <mergeCell ref="X38:AA38"/>
+    <mergeCell ref="AB38:AE38"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="F39:G39"/>
+    <mergeCell ref="H39:I39"/>
+    <mergeCell ref="J39:M39"/>
+    <mergeCell ref="N39:P39"/>
+    <mergeCell ref="T39:W39"/>
+    <mergeCell ref="X39:AA39"/>
+    <mergeCell ref="AB39:AE39"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="F40:G40"/>
+    <mergeCell ref="H40:I40"/>
+    <mergeCell ref="J40:M40"/>
+    <mergeCell ref="N40:P40"/>
+    <mergeCell ref="T40:W40"/>
+    <mergeCell ref="X40:AA40"/>
+    <mergeCell ref="AB40:AE40"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="H41:I41"/>
+    <mergeCell ref="J41:M41"/>
+    <mergeCell ref="N41:P41"/>
+    <mergeCell ref="T41:W41"/>
+    <mergeCell ref="X41:AA41"/>
+    <mergeCell ref="AB41:AE41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="F42:G42"/>
+    <mergeCell ref="H42:I42"/>
+    <mergeCell ref="J42:M42"/>
+    <mergeCell ref="N42:P42"/>
+    <mergeCell ref="T42:W42"/>
+    <mergeCell ref="X42:AA42"/>
+    <mergeCell ref="AB42:AE42"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="F43:G43"/>
+    <mergeCell ref="H43:I43"/>
+    <mergeCell ref="J43:M43"/>
+    <mergeCell ref="N43:P43"/>
+    <mergeCell ref="T43:W43"/>
+    <mergeCell ref="X43:AA43"/>
+    <mergeCell ref="AB43:AE43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="F44:G44"/>
+    <mergeCell ref="H44:I44"/>
+    <mergeCell ref="J44:M44"/>
+    <mergeCell ref="N44:P44"/>
+    <mergeCell ref="T44:W44"/>
+    <mergeCell ref="X44:AA44"/>
+    <mergeCell ref="AB44:AE44"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="F45:G45"/>
+    <mergeCell ref="H45:I45"/>
+    <mergeCell ref="J45:M45"/>
+    <mergeCell ref="N45:P45"/>
+    <mergeCell ref="T45:W45"/>
+    <mergeCell ref="X45:AA45"/>
+    <mergeCell ref="AB45:AE45"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="F46:G46"/>
+    <mergeCell ref="H46:I46"/>
+    <mergeCell ref="J46:M46"/>
+    <mergeCell ref="N46:P46"/>
+    <mergeCell ref="T46:W46"/>
+    <mergeCell ref="X46:AA46"/>
+    <mergeCell ref="AB46:AE46"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="F47:G47"/>
+    <mergeCell ref="H47:I47"/>
+    <mergeCell ref="J47:M47"/>
+    <mergeCell ref="N47:P47"/>
+    <mergeCell ref="T47:W47"/>
+    <mergeCell ref="X47:AA47"/>
+    <mergeCell ref="AB47:AE47"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="F48:G48"/>
+    <mergeCell ref="H48:I48"/>
+    <mergeCell ref="J48:M48"/>
+    <mergeCell ref="N48:P48"/>
+    <mergeCell ref="T48:W48"/>
+    <mergeCell ref="X48:AA48"/>
+    <mergeCell ref="AB48:AE48"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="F49:G49"/>
+    <mergeCell ref="H49:I49"/>
+    <mergeCell ref="J49:M49"/>
+    <mergeCell ref="N49:P49"/>
+    <mergeCell ref="T49:W49"/>
+    <mergeCell ref="X49:AA49"/>
+    <mergeCell ref="AB49:AE49"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="F50:G50"/>
+    <mergeCell ref="H50:I50"/>
+    <mergeCell ref="J50:M50"/>
+    <mergeCell ref="N50:P50"/>
+    <mergeCell ref="T50:W50"/>
+    <mergeCell ref="X50:AA50"/>
+    <mergeCell ref="AB50:AE50"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="F51:G51"/>
+    <mergeCell ref="H51:I51"/>
+    <mergeCell ref="J51:M51"/>
+    <mergeCell ref="N51:P51"/>
+    <mergeCell ref="T51:W51"/>
+    <mergeCell ref="X51:AA51"/>
+    <mergeCell ref="AB51:AE51"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="F52:G52"/>
+    <mergeCell ref="H52:I52"/>
+    <mergeCell ref="J52:M52"/>
+    <mergeCell ref="N52:P52"/>
+    <mergeCell ref="T52:W52"/>
+    <mergeCell ref="X52:AA52"/>
+    <mergeCell ref="AB52:AE52"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="F53:G53"/>
+    <mergeCell ref="H53:I53"/>
+    <mergeCell ref="J53:M53"/>
+    <mergeCell ref="N53:P53"/>
+    <mergeCell ref="T53:W53"/>
+    <mergeCell ref="X53:AA53"/>
+    <mergeCell ref="AB53:AE53"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="F54:G54"/>
+    <mergeCell ref="H54:I54"/>
+    <mergeCell ref="J54:M54"/>
+    <mergeCell ref="N54:P54"/>
+    <mergeCell ref="T54:W54"/>
+    <mergeCell ref="X54:AA54"/>
+    <mergeCell ref="AB54:AE54"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="F55:G55"/>
+    <mergeCell ref="H55:I55"/>
+    <mergeCell ref="J55:M55"/>
+    <mergeCell ref="N55:P55"/>
+    <mergeCell ref="T55:W55"/>
+    <mergeCell ref="X55:AA55"/>
+    <mergeCell ref="AB55:AE55"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="F56:G56"/>
+    <mergeCell ref="H56:I56"/>
+    <mergeCell ref="J56:M56"/>
+    <mergeCell ref="N56:P56"/>
+    <mergeCell ref="T56:W56"/>
+    <mergeCell ref="X56:AA56"/>
+    <mergeCell ref="AB56:AE56"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="F57:G57"/>
+    <mergeCell ref="H57:I57"/>
+    <mergeCell ref="J57:M57"/>
+    <mergeCell ref="N57:P57"/>
+    <mergeCell ref="T57:W57"/>
+    <mergeCell ref="X57:AA57"/>
+    <mergeCell ref="AB57:AE57"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="F58:G58"/>
+    <mergeCell ref="H58:I58"/>
+    <mergeCell ref="J58:M58"/>
+    <mergeCell ref="N58:P58"/>
+    <mergeCell ref="T58:W58"/>
+    <mergeCell ref="X58:AA58"/>
+    <mergeCell ref="AB58:AE58"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="F59:G59"/>
+    <mergeCell ref="H59:I59"/>
+    <mergeCell ref="J59:M59"/>
+    <mergeCell ref="N59:P59"/>
+    <mergeCell ref="T59:W59"/>
+    <mergeCell ref="X59:AA59"/>
+    <mergeCell ref="AB59:AE59"/>
+    <mergeCell ref="B60:C60"/>
+    <mergeCell ref="F60:G60"/>
+    <mergeCell ref="H60:I60"/>
+    <mergeCell ref="J60:M60"/>
+    <mergeCell ref="N60:P60"/>
+    <mergeCell ref="T60:W60"/>
+    <mergeCell ref="X60:AA60"/>
+    <mergeCell ref="AB60:AE60"/>
     <mergeCell ref="O2:T2"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="F10:G10"/>

</xml_diff>